<commit_message>
update maps and code
</commit_message>
<xml_diff>
--- a/results/RR/reg_tables_formatted.xlsx
+++ b/results/RR/reg_tables_formatted.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihzhang/Documents/GitHub/psid-rs/results/RR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C570A96-9657-A348-87A9-BB71744C67B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD0CDC5-7B67-CE48-A215-38E4A9A160FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22880" windowHeight="16580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="314">
   <si>
     <t>2a</t>
   </si>
@@ -2999,8 +2999,63 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>&lt; 0.01; Other racial groups included in sample but omitted here</t>
-    </r>
+      <t>&lt; 0.01 (two-tailed tests)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt; 0.05; **</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt; 0.01 (two-tailed tests) </t>
+    </r>
+  </si>
+  <si>
+    <t>Other racial groups included in sample but omitted here</t>
   </si>
 </sst>
 </file>
@@ -3009,8 +3064,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00_);\(0.00\)"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.000_);\(0.000\)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000_);\(0.000\)"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -3131,26 +3186,26 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3181,36 +3236,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3492,10 +3547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G205"/>
+  <dimension ref="A1:G207"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E206" sqref="E206"/>
+    <sheetView topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152:C207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" customHeight="1"/>
@@ -3507,10 +3562,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" customHeight="1">
       <c r="A1" s="3"/>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="31"/>
+      <c r="C1" s="40"/>
     </row>
     <row r="2" spans="1:3" ht="16" customHeight="1" thickBot="1">
       <c r="A2" s="19"/>
@@ -4750,525 +4805,542 @@
         <v>-2.1640000000000001</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="16" customHeight="1">
-      <c r="A152" s="5" t="s">
+    <row r="152" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
+      <c r="A152" s="3"/>
+      <c r="B152" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C152" s="40"/>
+    </row>
+    <row r="153" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1" thickBot="1">
+      <c r="A153" s="19"/>
+      <c r="B153" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C153" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="16" customHeight="1">
+      <c r="A154" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B152" s="9"/>
-      <c r="C152" s="9"/>
-    </row>
-    <row r="153" spans="1:3" ht="16" customHeight="1">
-      <c r="A153" s="9" t="s">
+      <c r="B154" s="9"/>
+      <c r="C154" s="9"/>
+    </row>
+    <row r="155" spans="1:3" ht="16" customHeight="1">
+      <c r="A155" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B153" s="26" t="s">
+      <c r="B155" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C153" s="26" t="s">
+      <c r="C155" s="26" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="154" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
-      <c r="A154" s="4"/>
-      <c r="B154" s="27">
+    <row r="156" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
+      <c r="A156" s="4"/>
+      <c r="B156" s="27">
         <v>-2.8000000000000001E-2</v>
       </c>
-      <c r="C154" s="27">
+      <c r="C156" s="27">
         <v>-2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="16" customHeight="1">
-      <c r="A155" s="1" t="s">
+    <row r="157" spans="1:3" ht="16" customHeight="1">
+      <c r="A157" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B155" s="9"/>
-      <c r="C155" s="9"/>
-    </row>
-    <row r="156" spans="1:3" ht="16" customHeight="1">
-      <c r="A156" s="10" t="s">
+      <c r="B157" s="9"/>
+      <c r="C157" s="9"/>
+    </row>
+    <row r="158" spans="1:3" ht="16" customHeight="1">
+      <c r="A158" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B156" s="26" t="s">
+      <c r="B158" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="C156" s="26" t="s">
+      <c r="C158" s="26" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
-      <c r="A157" s="4"/>
-      <c r="B157" s="27">
-        <v>-2.9000000000000001E-2</v>
-      </c>
-      <c r="C157" s="27">
-        <v>-2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="16" customHeight="1">
-      <c r="A158" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B158" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C158" s="26" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="159" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
       <c r="A159" s="4"/>
       <c r="B159" s="27">
+        <v>-2.9000000000000001E-2</v>
+      </c>
+      <c r="C159" s="27">
+        <v>-2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="16" customHeight="1">
+      <c r="A160" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B160" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="C160" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
+      <c r="A161" s="4"/>
+      <c r="B161" s="27">
         <v>-6.3E-2</v>
       </c>
-      <c r="C159" s="27">
+      <c r="C161" s="27">
         <v>-6.3E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="16" customHeight="1">
-      <c r="A160" s="1" t="s">
+    <row r="162" spans="1:3" ht="16" customHeight="1">
+      <c r="A162" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B160" s="9"/>
-      <c r="C160" s="9"/>
-    </row>
-    <row r="161" spans="1:3" ht="16" customHeight="1">
-      <c r="A161" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B161" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="C161" s="26" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
-      <c r="A162" s="4"/>
-      <c r="B162" s="27">
-        <v>-2.8000000000000001E-2</v>
-      </c>
-      <c r="C162" s="27">
-        <v>-2.8000000000000001E-2</v>
-      </c>
+      <c r="B162" s="9"/>
+      <c r="C162" s="9"/>
     </row>
     <row r="163" spans="1:3" ht="16" customHeight="1">
       <c r="A163" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B163" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C163" s="26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="164" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
       <c r="A164" s="4"/>
       <c r="B164" s="27">
-        <v>-5.2999999999999999E-2</v>
+        <v>-2.8000000000000001E-2</v>
       </c>
       <c r="C164" s="27">
-        <v>-5.2999999999999999E-2</v>
+        <v>-2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="16" customHeight="1">
       <c r="A165" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B165" s="26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C165" s="26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="166" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
       <c r="A166" s="4"/>
       <c r="B166" s="27">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="C166" s="27">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="16" customHeight="1">
+      <c r="A167" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B167" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C167" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
+      <c r="A168" s="4"/>
+      <c r="B168" s="27">
         <v>-8.2000000000000003E-2</v>
       </c>
-      <c r="C166" s="27">
+      <c r="C168" s="27">
         <v>-0.152</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="16" customHeight="1">
-      <c r="A167" s="1" t="s">
+    <row r="169" spans="1:3" ht="16" customHeight="1">
+      <c r="A169" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B167" s="9"/>
-      <c r="C167" s="9"/>
-    </row>
-    <row r="168" spans="1:3" ht="16" customHeight="1">
-      <c r="A168" s="9" t="s">
+      <c r="B169" s="9"/>
+      <c r="C169" s="9"/>
+    </row>
+    <row r="170" spans="1:3" ht="16" customHeight="1">
+      <c r="A170" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B168" s="26" t="s">
+      <c r="B170" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="C168" s="26" t="s">
+      <c r="C170" s="26" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="169" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
-      <c r="A169" s="4"/>
-      <c r="B169" s="27">
+    <row r="171" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
+      <c r="A171" s="4"/>
+      <c r="B171" s="27">
         <v>-0.04</v>
       </c>
-      <c r="C169" s="27">
+      <c r="C171" s="27">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="16" customHeight="1">
-      <c r="A170" s="1" t="s">
+    <row r="172" spans="1:3" ht="16" customHeight="1">
+      <c r="A172" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B170" s="9"/>
-      <c r="C170" s="9"/>
-    </row>
-    <row r="171" spans="1:3" ht="16" customHeight="1">
-      <c r="A171" s="9" t="s">
+      <c r="B172" s="9"/>
+      <c r="C172" s="9"/>
+    </row>
+    <row r="173" spans="1:3" ht="16" customHeight="1">
+      <c r="A173" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B171" s="26" t="s">
+      <c r="B173" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="C171" s="26" t="s">
+      <c r="C173" s="26" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="172" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
-      <c r="A172" s="4"/>
-      <c r="B172" s="27">
+    <row r="174" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
+      <c r="A174" s="4"/>
+      <c r="B174" s="27">
         <v>-2.7E-2</v>
       </c>
-      <c r="C172" s="27">
+      <c r="C174" s="27">
         <v>-2.7E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="16" customHeight="1">
-      <c r="A173" s="1" t="s">
+    <row r="175" spans="1:3" ht="16" customHeight="1">
+      <c r="A175" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B173" s="9"/>
-      <c r="C173" s="9"/>
-    </row>
-    <row r="174" spans="1:3" ht="16" customHeight="1">
-      <c r="A174" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B174" s="26">
-        <v>0.78400000000000003</v>
-      </c>
-      <c r="C174" s="26">
-        <v>0.77800000000000002</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
-      <c r="A175" s="10"/>
-      <c r="B175" s="27">
-        <v>-0.745</v>
-      </c>
-      <c r="C175" s="27">
-        <v>-0.749</v>
-      </c>
+      <c r="B175" s="9"/>
+      <c r="C175" s="9"/>
     </row>
     <row r="176" spans="1:3" ht="16" customHeight="1">
       <c r="A176" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B176" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="C176" s="26" t="s">
-        <v>156</v>
+        <v>17</v>
+      </c>
+      <c r="B176" s="26">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="C176" s="26">
+        <v>0.77800000000000002</v>
       </c>
     </row>
     <row r="177" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
       <c r="A177" s="10"/>
       <c r="B177" s="27">
-        <v>-4.3999999999999997E-2</v>
+        <v>-0.745</v>
       </c>
       <c r="C177" s="27">
-        <v>-4.3999999999999997E-2</v>
+        <v>-0.749</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="16" customHeight="1">
       <c r="A178" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B178" s="26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C178" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="179" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
       <c r="A179" s="10"/>
       <c r="B179" s="27">
-        <v>-4.8000000000000001E-2</v>
+        <v>-4.3999999999999997E-2</v>
       </c>
       <c r="C179" s="27">
-        <v>-4.8000000000000001E-2</v>
+        <v>-4.3999999999999997E-2</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="16" customHeight="1">
       <c r="A180" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B180" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C180" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="181" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
       <c r="A181" s="10"/>
       <c r="B181" s="27">
-        <v>-0.05</v>
+        <v>-4.8000000000000001E-2</v>
       </c>
       <c r="C181" s="27">
-        <v>-0.05</v>
+        <v>-4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="16" customHeight="1">
       <c r="A182" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B182" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C182" s="26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="183" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
       <c r="A183" s="10"/>
       <c r="B183" s="27">
-        <v>-5.6000000000000001E-2</v>
+        <v>-0.05</v>
       </c>
       <c r="C183" s="27">
-        <v>-5.6000000000000001E-2</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="16" customHeight="1">
       <c r="A184" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B184" s="26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C184" s="26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="185" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
       <c r="A185" s="10"/>
       <c r="B185" s="27">
-        <v>-5.8999999999999997E-2</v>
+        <v>-5.6000000000000001E-2</v>
       </c>
       <c r="C185" s="27">
-        <v>-0.06</v>
+        <v>-5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="16" customHeight="1">
       <c r="A186" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B186" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C186" s="26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
+      <c r="A187" s="10"/>
+      <c r="B187" s="27">
+        <v>-5.8999999999999997E-2</v>
+      </c>
+      <c r="C187" s="27">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="16" customHeight="1">
+      <c r="A188" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B186" s="26">
+      <c r="B188" s="26">
         <v>-0.73899999999999999</v>
       </c>
-      <c r="C186" s="26">
+      <c r="C188" s="26">
         <v>-0.82399999999999995</v>
       </c>
     </row>
-    <row r="187" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
-      <c r="A187" s="4"/>
-      <c r="B187" s="27">
+    <row r="189" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
+      <c r="A189" s="4"/>
+      <c r="B189" s="27">
         <v>-0.65200000000000002</v>
       </c>
-      <c r="C187" s="27">
+      <c r="C189" s="27">
         <v>-0.68200000000000005</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="16" customHeight="1">
-      <c r="A188" s="1" t="s">
+    <row r="190" spans="1:3" ht="16" customHeight="1">
+      <c r="A190" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B188" s="9"/>
-      <c r="C188" s="9"/>
-    </row>
-    <row r="189" spans="1:3" ht="16" customHeight="1">
-      <c r="A189" s="9" t="s">
+      <c r="B190" s="9"/>
+      <c r="C190" s="9"/>
+    </row>
+    <row r="191" spans="1:3" ht="16" customHeight="1">
+      <c r="A191" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B189" s="26" t="s">
+      <c r="B191" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="C189" s="26" t="s">
+      <c r="C191" s="26" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="190" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
-      <c r="A190" s="4"/>
-      <c r="B190" s="27">
+    <row r="192" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
+      <c r="A192" s="4"/>
+      <c r="B192" s="27">
         <v>-2.7E-2</v>
       </c>
-      <c r="C190" s="27">
+      <c r="C192" s="27">
         <v>-2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:3" s="12" customFormat="1" ht="16" customHeight="1">
-      <c r="A191" s="9" t="s">
+    <row r="193" spans="1:3" s="12" customFormat="1" ht="16" customHeight="1">
+      <c r="A193" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B191" s="26">
+      <c r="B193" s="26">
         <v>0.315</v>
       </c>
-      <c r="C191" s="26">
+      <c r="C193" s="26">
         <v>0.314</v>
       </c>
     </row>
-    <row r="192" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
-      <c r="B192" s="27">
+    <row r="194" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
+      <c r="B194" s="27">
         <v>-0.20699999999999999</v>
       </c>
-      <c r="C192" s="27">
+      <c r="C194" s="27">
         <v>-0.21</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="16" customHeight="1">
-      <c r="A193" s="1" t="s">
+    <row r="195" spans="1:3" ht="16" customHeight="1">
+      <c r="A195" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B193" s="9"/>
-      <c r="C193" s="9"/>
-    </row>
-    <row r="194" spans="1:3" s="12" customFormat="1" ht="16" customHeight="1">
-      <c r="A194" s="9" t="s">
+      <c r="B195" s="9"/>
+      <c r="C195" s="9"/>
+    </row>
+    <row r="196" spans="1:3" s="12" customFormat="1" ht="16" customHeight="1">
+      <c r="A196" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B194" s="26" t="s">
+      <c r="B196" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="C194" s="26" t="s">
+      <c r="C196" s="26" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="195" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
-      <c r="B195" s="27">
+    <row r="197" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
+      <c r="B197" s="27">
         <v>-2.9000000000000001E-2</v>
       </c>
-      <c r="C195" s="27">
+      <c r="C197" s="27">
         <v>-2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="16" customHeight="1">
-      <c r="A196" s="9" t="s">
+    <row r="198" spans="1:3" ht="16" customHeight="1">
+      <c r="A198" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B196" s="26">
+      <c r="B198" s="26">
         <v>1E-3</v>
       </c>
-      <c r="C196" s="26">
+      <c r="C198" s="26">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="197" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
-      <c r="A197" s="4"/>
-      <c r="B197" s="27">
+    <row r="199" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1">
+      <c r="A199" s="4"/>
+      <c r="B199" s="27">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="C197" s="27">
+      <c r="C199" s="27">
         <v>-3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="198" spans="1:3" s="12" customFormat="1" ht="16" customHeight="1">
-      <c r="A198" s="11" t="s">
+    <row r="200" spans="1:3" s="12" customFormat="1" ht="16" customHeight="1">
+      <c r="A200" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B198" s="14" t="s">
+      <c r="B200" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C198" s="14" t="s">
+      <c r="C200" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="199" spans="1:3" s="12" customFormat="1" ht="16" customHeight="1">
-      <c r="A199" s="11" t="s">
+    <row r="201" spans="1:3" s="12" customFormat="1" ht="16" customHeight="1">
+      <c r="A201" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B199" s="14" t="s">
+      <c r="B201" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C199" s="14" t="s">
+      <c r="C201" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="16" customHeight="1">
-      <c r="A200" s="1" t="s">
+    <row r="202" spans="1:3" ht="16" customHeight="1">
+      <c r="A202" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B200" s="26" t="s">
+      <c r="B202" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="C200" s="26" t="s">
+      <c r="C202" s="26" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="201" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1" thickBot="1">
-      <c r="A201" s="25"/>
-      <c r="B201" s="28">
+    <row r="203" spans="1:3" s="8" customFormat="1" ht="16" customHeight="1" thickBot="1">
+      <c r="A203" s="25"/>
+      <c r="B203" s="28">
         <v>-8.1000000000000003E-2</v>
       </c>
-      <c r="C201" s="28">
+      <c r="C203" s="28">
         <v>-9.4E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="16" customHeight="1">
-      <c r="A202" s="3" t="s">
+    <row r="204" spans="1:3" ht="16" customHeight="1">
+      <c r="A204" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B202" s="22">
+      <c r="B204" s="22">
         <v>56292</v>
       </c>
-      <c r="C202" s="22">
+      <c r="C204" s="22">
         <v>56292</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="16" customHeight="1">
-      <c r="A203" s="3" t="s">
+    <row r="205" spans="1:3" ht="16" customHeight="1">
+      <c r="A205" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B203" s="21">
+      <c r="B205" s="21">
         <v>0.308</v>
       </c>
-      <c r="C203" s="21">
+      <c r="C205" s="21">
         <v>0.308</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="16" customHeight="1" thickBot="1">
-      <c r="A204" s="3" t="s">
+    <row r="206" spans="1:3" ht="16" customHeight="1" thickBot="1">
+      <c r="A206" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B204" s="23">
+      <c r="B206" s="23">
         <v>-26766.6</v>
       </c>
-      <c r="C204" s="23">
+      <c r="C206" s="23">
         <v>-26792.01</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="16" customHeight="1">
-      <c r="A205" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B205" s="17"/>
-      <c r="C205" s="17"/>
+    <row r="207" spans="1:3" ht="16" customHeight="1">
+      <c r="A207" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B207" s="17"/>
+      <c r="C207" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B152:C152"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5292,10 +5364,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" customHeight="1">
       <c r="A1" s="3"/>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="31"/>
+      <c r="C1" s="40"/>
     </row>
     <row r="2" spans="1:3" ht="16" customHeight="1" thickBot="1">
       <c r="A2" s="19"/>
@@ -6278,8 +6350,8 @@
       <c r="A108" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B108" s="32"/>
-      <c r="C108" s="32"/>
+      <c r="B108" s="41"/>
+      <c r="C108" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6293,10 +6365,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F20AB4-393E-1541-B39E-13DC501AEEFA}">
-  <dimension ref="A1:R218"/>
+  <dimension ref="A1:R216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="K155" sqref="K155"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A154" sqref="A154:G211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" customHeight="1"/>
@@ -6308,14 +6380,14 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" customHeight="1">
       <c r="A1" s="3"/>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1" thickBot="1">
       <c r="A2" s="19"/>
@@ -6325,16 +6397,16 @@
       <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="39" t="s">
         <v>81</v>
       </c>
     </row>
@@ -6370,22 +6442,22 @@
     </row>
     <row r="5" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A5" s="13"/>
-      <c r="B5" s="38">
+      <c r="B5" s="36">
         <v>-0.02</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="36">
         <v>-5.3999999999999999E-2</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="36">
         <v>-0.499</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="36">
         <v>-1.4690000000000001</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="36">
         <v>-0.52400000000000002</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="36">
         <v>-1.1919999999999999</v>
       </c>
     </row>
@@ -6414,22 +6486,22 @@
     </row>
     <row r="7" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A7" s="13"/>
-      <c r="B7" s="38">
+      <c r="B7" s="36">
         <v>-3.1E-2</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="36">
         <v>-7.8E-2</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="36">
         <v>-0.745</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="36">
         <v>-2.323</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="36">
         <v>-0.67500000000000004</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="36">
         <v>-1.998</v>
       </c>
     </row>
@@ -6458,22 +6530,22 @@
     </row>
     <row r="9" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A9" s="13"/>
-      <c r="B9" s="38">
+      <c r="B9" s="36">
         <v>-0.08</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="36">
         <v>-0.20699999999999999</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="36">
         <v>-1.59</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="36">
         <v>-6.5609999999999999</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="36">
         <v>-1.379</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="36">
         <v>-4.63</v>
       </c>
     </row>
@@ -6502,22 +6574,22 @@
     </row>
     <row r="11" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A11" s="13"/>
-      <c r="B11" s="38">
+      <c r="B11" s="36">
         <v>-6.7000000000000004E-2</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="36">
         <v>-0.13900000000000001</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="36">
         <v>-1.748</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="36">
         <v>-5.952</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="36">
         <v>-1.335</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="36">
         <v>-4.524</v>
       </c>
     </row>
@@ -6546,22 +6618,22 @@
     </row>
     <row r="13" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A13" s="13"/>
-      <c r="B13" s="38">
+      <c r="B13" s="36">
         <v>-0.107</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="36">
         <v>-0.19400000000000001</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="36">
         <v>-2.2959999999999998</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="36">
         <v>-4.0129999999999999</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="36">
         <v>-2.2770000000000001</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G13" s="36">
         <v>-3.286</v>
       </c>
     </row>
@@ -6571,10 +6643,10 @@
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
     </row>
     <row r="15" spans="1:7" ht="16" customHeight="1">
       <c r="A15" s="9" t="s">
@@ -6601,22 +6673,22 @@
     </row>
     <row r="16" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A16" s="11"/>
-      <c r="B16" s="38">
+      <c r="B16" s="36">
         <v>-2.9000000000000001E-2</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="36">
         <v>-0.105</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="36">
         <v>-0.77500000000000002</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="36">
         <v>-2.4300000000000002</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16" s="36">
         <v>-0.68400000000000005</v>
       </c>
-      <c r="G16" s="38">
+      <c r="G16" s="36">
         <v>-1.8779999999999999</v>
       </c>
     </row>
@@ -6645,22 +6717,22 @@
     </row>
     <row r="18" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A18" s="11"/>
-      <c r="B18" s="38">
+      <c r="B18" s="36">
         <v>-1.6E-2</v>
       </c>
-      <c r="C18" s="38">
+      <c r="C18" s="36">
         <v>-5.5E-2</v>
       </c>
-      <c r="D18" s="38">
+      <c r="D18" s="36">
         <v>-0.49</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E18" s="36">
         <v>-1.4279999999999999</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="36">
         <v>-0.42199999999999999</v>
       </c>
-      <c r="G18" s="38">
+      <c r="G18" s="36">
         <v>-1.0309999999999999</v>
       </c>
     </row>
@@ -6670,8 +6742,8 @@
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
     </row>
@@ -6700,22 +6772,22 @@
     </row>
     <row r="21" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A21" s="11"/>
-      <c r="B21" s="38">
+      <c r="B21" s="36">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="C21" s="38">
+      <c r="C21" s="36">
         <v>-7.1999999999999995E-2</v>
       </c>
-      <c r="D21" s="38">
+      <c r="D21" s="36">
         <v>-0.441</v>
       </c>
-      <c r="E21" s="38">
+      <c r="E21" s="36">
         <v>-1.859</v>
       </c>
-      <c r="F21" s="38">
+      <c r="F21" s="36">
         <v>-0.38100000000000001</v>
       </c>
-      <c r="G21" s="38">
+      <c r="G21" s="36">
         <v>-1.4119999999999999</v>
       </c>
     </row>
@@ -6744,22 +6816,22 @@
     </row>
     <row r="23" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A23" s="11"/>
-      <c r="B23" s="38">
+      <c r="B23" s="36">
         <v>-2.1000000000000001E-2</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C23" s="36">
         <v>-8.1000000000000003E-2</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="36">
         <v>-0.53900000000000003</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="36">
         <v>-2.0379999999999998</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="36">
         <v>-0.45500000000000002</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="36">
         <v>-1.4239999999999999</v>
       </c>
     </row>
@@ -6788,22 +6860,22 @@
     </row>
     <row r="25" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A25" s="11"/>
-      <c r="B25" s="38">
+      <c r="B25" s="36">
         <v>-2.7E-2</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C25" s="36">
         <v>-9.5000000000000001E-2</v>
       </c>
-      <c r="D25" s="38">
+      <c r="D25" s="36">
         <v>-0.63400000000000001</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="36">
         <v>-2.5310000000000001</v>
       </c>
-      <c r="F25" s="38">
+      <c r="F25" s="36">
         <v>-0.51100000000000001</v>
       </c>
-      <c r="G25" s="38">
+      <c r="G25" s="36">
         <v>-1.7729999999999999</v>
       </c>
     </row>
@@ -6813,10 +6885,10 @@
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" spans="1:7" ht="16" customHeight="1">
       <c r="A27" s="9" t="s">
@@ -6837,16 +6909,16 @@
     </row>
     <row r="28" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A28" s="11"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38">
+      <c r="B28" s="36"/>
+      <c r="C28" s="36">
         <v>-0.114</v>
       </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38">
+      <c r="D28" s="36"/>
+      <c r="E28" s="36">
         <v>-2.762</v>
       </c>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38">
+      <c r="F28" s="36"/>
+      <c r="G28" s="36">
         <v>-2.3119999999999998</v>
       </c>
     </row>
@@ -6869,16 +6941,16 @@
     </row>
     <row r="30" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A30" s="11"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38">
+      <c r="B30" s="36"/>
+      <c r="C30" s="36">
         <v>-6.0999999999999999E-2</v>
       </c>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38">
+      <c r="D30" s="36"/>
+      <c r="E30" s="36">
         <v>-1.6339999999999999</v>
       </c>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38">
+      <c r="F30" s="36"/>
+      <c r="G30" s="36">
         <v>-1.296</v>
       </c>
     </row>
@@ -6901,16 +6973,16 @@
     </row>
     <row r="32" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A32" s="11"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38">
+      <c r="B32" s="36"/>
+      <c r="C32" s="36">
         <v>-0.158</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38">
+      <c r="D32" s="36"/>
+      <c r="E32" s="36">
         <v>-4.96</v>
       </c>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38">
+      <c r="F32" s="36"/>
+      <c r="G32" s="36">
         <v>-3.9769999999999999</v>
       </c>
     </row>
@@ -6933,16 +7005,16 @@
     </row>
     <row r="34" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A34" s="11"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38">
+      <c r="B34" s="36"/>
+      <c r="C34" s="36">
         <v>-9.2999999999999999E-2</v>
       </c>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38">
+      <c r="D34" s="36"/>
+      <c r="E34" s="36">
         <v>-2.8610000000000002</v>
       </c>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38">
+      <c r="F34" s="36"/>
+      <c r="G34" s="36">
         <v>-2.39</v>
       </c>
     </row>
@@ -6965,16 +7037,16 @@
     </row>
     <row r="36" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A36" s="11"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38">
+      <c r="B36" s="36"/>
+      <c r="C36" s="36">
         <v>-0.24199999999999999</v>
       </c>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38">
+      <c r="D36" s="36"/>
+      <c r="E36" s="36">
         <v>-7.2649999999999997</v>
       </c>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38">
+      <c r="F36" s="36"/>
+      <c r="G36" s="36">
         <v>-5.1520000000000001</v>
       </c>
     </row>
@@ -6997,16 +7069,16 @@
     </row>
     <row r="38" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A38" s="13"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38">
+      <c r="B38" s="36"/>
+      <c r="C38" s="36">
         <v>-0.25700000000000001</v>
       </c>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38">
+      <c r="D38" s="36"/>
+      <c r="E38" s="36">
         <v>-7.5439999999999996</v>
       </c>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38">
+      <c r="F38" s="36"/>
+      <c r="G38" s="36">
         <v>-5.49</v>
       </c>
     </row>
@@ -7029,16 +7101,16 @@
     </row>
     <row r="40" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A40" s="11"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38">
+      <c r="B40" s="36"/>
+      <c r="C40" s="36">
         <v>-0.50600000000000001</v>
       </c>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38">
+      <c r="D40" s="36"/>
+      <c r="E40" s="36">
         <v>-11.865</v>
       </c>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38">
+      <c r="F40" s="36"/>
+      <c r="G40" s="36">
         <v>-7.0490000000000004</v>
       </c>
     </row>
@@ -7061,16 +7133,16 @@
     </row>
     <row r="42" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A42" s="13"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38">
+      <c r="B42" s="36"/>
+      <c r="C42" s="36">
         <v>-0.19700000000000001</v>
       </c>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38">
+      <c r="D42" s="36"/>
+      <c r="E42" s="36">
         <v>-6.3659999999999997</v>
       </c>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38">
+      <c r="F42" s="36"/>
+      <c r="G42" s="36">
         <v>-4.8179999999999996</v>
       </c>
     </row>
@@ -7093,16 +7165,16 @@
     </row>
     <row r="44" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A44" s="13"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38">
+      <c r="B44" s="36"/>
+      <c r="C44" s="36">
         <v>-0.219</v>
       </c>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38">
+      <c r="D44" s="36"/>
+      <c r="E44" s="36">
         <v>-8.06</v>
       </c>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38">
+      <c r="F44" s="36"/>
+      <c r="G44" s="36">
         <v>-16.984999999999999</v>
       </c>
     </row>
@@ -7125,16 +7197,16 @@
     </row>
     <row r="46" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A46" s="13"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38">
+      <c r="B46" s="36"/>
+      <c r="C46" s="36">
         <v>-0.248</v>
       </c>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38">
+      <c r="D46" s="36"/>
+      <c r="E46" s="36">
         <v>-8.3539999999999992</v>
       </c>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38">
+      <c r="F46" s="36"/>
+      <c r="G46" s="36">
         <v>-5.3390000000000004</v>
       </c>
     </row>
@@ -7144,10 +7216,10 @@
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="35"/>
     </row>
     <row r="48" spans="1:7" ht="16" customHeight="1">
       <c r="A48" s="9" t="s">
@@ -7168,16 +7240,16 @@
     </row>
     <row r="49" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A49" s="11"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38">
+      <c r="B49" s="36"/>
+      <c r="C49" s="36">
         <v>-7.9000000000000001E-2</v>
       </c>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38">
+      <c r="D49" s="36"/>
+      <c r="E49" s="36">
         <v>-2.0960000000000001</v>
       </c>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38">
+      <c r="F49" s="36"/>
+      <c r="G49" s="36">
         <v>-1.7290000000000001</v>
       </c>
     </row>
@@ -7200,16 +7272,16 @@
     </row>
     <row r="51" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A51" s="11"/>
-      <c r="B51" s="38"/>
-      <c r="C51" s="38">
+      <c r="B51" s="36"/>
+      <c r="C51" s="36">
         <v>-9.0999999999999998E-2</v>
       </c>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38">
+      <c r="D51" s="36"/>
+      <c r="E51" s="36">
         <v>-2.5459999999999998</v>
       </c>
-      <c r="F51" s="38"/>
-      <c r="G51" s="38">
+      <c r="F51" s="36"/>
+      <c r="G51" s="36">
         <v>-2.0350000000000001</v>
       </c>
     </row>
@@ -7232,16 +7304,16 @@
     </row>
     <row r="53" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A53" s="11"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38">
+      <c r="B53" s="36"/>
+      <c r="C53" s="36">
         <v>-0.14099999999999999</v>
       </c>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38">
+      <c r="D53" s="36"/>
+      <c r="E53" s="36">
         <v>-3.8460000000000001</v>
       </c>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38">
+      <c r="F53" s="36"/>
+      <c r="G53" s="36">
         <v>-3.5190000000000001</v>
       </c>
     </row>
@@ -7264,16 +7336,16 @@
     </row>
     <row r="55" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A55" s="11"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="38">
+      <c r="B55" s="36"/>
+      <c r="C55" s="36">
         <v>-0.129</v>
       </c>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38">
+      <c r="D55" s="36"/>
+      <c r="E55" s="36">
         <v>-3.367</v>
       </c>
-      <c r="F55" s="38"/>
-      <c r="G55" s="38">
+      <c r="F55" s="36"/>
+      <c r="G55" s="36">
         <v>-2.778</v>
       </c>
     </row>
@@ -7296,16 +7368,16 @@
     </row>
     <row r="57" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A57" s="11"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="38">
+      <c r="B57" s="36"/>
+      <c r="C57" s="36">
         <v>-0.16300000000000001</v>
       </c>
-      <c r="D57" s="38"/>
-      <c r="E57" s="38">
+      <c r="D57" s="36"/>
+      <c r="E57" s="36">
         <v>-4.258</v>
       </c>
-      <c r="F57" s="38"/>
-      <c r="G57" s="38">
+      <c r="F57" s="36"/>
+      <c r="G57" s="36">
         <v>-3.589</v>
       </c>
     </row>
@@ -7328,16 +7400,16 @@
     </row>
     <row r="59" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A59" s="11"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="38">
+      <c r="B59" s="36"/>
+      <c r="C59" s="36">
         <v>-0.22</v>
       </c>
-      <c r="D59" s="38"/>
-      <c r="E59" s="38">
+      <c r="D59" s="36"/>
+      <c r="E59" s="36">
         <v>-7.7770000000000001</v>
       </c>
-      <c r="F59" s="38"/>
-      <c r="G59" s="38">
+      <c r="F59" s="36"/>
+      <c r="G59" s="36">
         <v>-6.1909999999999998</v>
       </c>
     </row>
@@ -7360,16 +7432,16 @@
     </row>
     <row r="61" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A61" s="11"/>
-      <c r="B61" s="38"/>
-      <c r="C61" s="38">
+      <c r="B61" s="36"/>
+      <c r="C61" s="36">
         <v>-0.28899999999999998</v>
       </c>
-      <c r="D61" s="38"/>
-      <c r="E61" s="38">
+      <c r="D61" s="36"/>
+      <c r="E61" s="36">
         <v>-8.9979999999999993</v>
       </c>
-      <c r="F61" s="38"/>
-      <c r="G61" s="38">
+      <c r="F61" s="36"/>
+      <c r="G61" s="36">
         <v>-7.056</v>
       </c>
     </row>
@@ -7392,16 +7464,16 @@
     </row>
     <row r="63" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A63" s="11"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="38">
+      <c r="B63" s="36"/>
+      <c r="C63" s="36">
         <v>-0.38400000000000001</v>
       </c>
-      <c r="D63" s="38"/>
-      <c r="E63" s="38">
+      <c r="D63" s="36"/>
+      <c r="E63" s="36">
         <v>-11.569000000000001</v>
       </c>
-      <c r="F63" s="38"/>
-      <c r="G63" s="38">
+      <c r="F63" s="36"/>
+      <c r="G63" s="36">
         <v>-7.5819999999999999</v>
       </c>
     </row>
@@ -7424,16 +7496,16 @@
     </row>
     <row r="65" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A65" s="11"/>
-      <c r="B65" s="38"/>
-      <c r="C65" s="38">
+      <c r="B65" s="36"/>
+      <c r="C65" s="36">
         <v>-0.22800000000000001</v>
       </c>
-      <c r="D65" s="38"/>
-      <c r="E65" s="38">
+      <c r="D65" s="36"/>
+      <c r="E65" s="36">
         <v>-4.5250000000000004</v>
       </c>
-      <c r="F65" s="38"/>
-      <c r="G65" s="38">
+      <c r="F65" s="36"/>
+      <c r="G65" s="36">
         <v>-3.8719999999999999</v>
       </c>
     </row>
@@ -7456,16 +7528,16 @@
     </row>
     <row r="67" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A67" s="11"/>
-      <c r="B67" s="38"/>
-      <c r="C67" s="38">
+      <c r="B67" s="36"/>
+      <c r="C67" s="36">
         <v>-0.29899999999999999</v>
       </c>
-      <c r="D67" s="38"/>
-      <c r="E67" s="38">
+      <c r="D67" s="36"/>
+      <c r="E67" s="36">
         <v>-9.92</v>
       </c>
-      <c r="F67" s="38"/>
-      <c r="G67" s="38">
+      <c r="F67" s="36"/>
+      <c r="G67" s="36">
         <v>-6.9610000000000003</v>
       </c>
     </row>
@@ -7488,16 +7560,16 @@
     </row>
     <row r="69" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A69" s="11"/>
-      <c r="B69" s="38"/>
-      <c r="C69" s="38">
+      <c r="B69" s="36"/>
+      <c r="C69" s="36">
         <v>-0.249</v>
       </c>
-      <c r="D69" s="38"/>
-      <c r="E69" s="38">
+      <c r="D69" s="36"/>
+      <c r="E69" s="36">
         <v>-10.997999999999999</v>
       </c>
-      <c r="F69" s="38"/>
-      <c r="G69" s="38">
+      <c r="F69" s="36"/>
+      <c r="G69" s="36">
         <v>-8.2420000000000009</v>
       </c>
     </row>
@@ -7520,16 +7592,16 @@
     </row>
     <row r="71" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A71" s="13"/>
-      <c r="B71" s="38"/>
-      <c r="C71" s="38">
+      <c r="B71" s="36"/>
+      <c r="C71" s="36">
         <v>-0.16700000000000001</v>
       </c>
-      <c r="D71" s="38"/>
-      <c r="E71" s="38">
+      <c r="D71" s="36"/>
+      <c r="E71" s="36">
         <v>-6.4180000000000001</v>
       </c>
-      <c r="F71" s="38"/>
-      <c r="G71" s="38">
+      <c r="F71" s="36"/>
+      <c r="G71" s="36">
         <v>-4.9139999999999997</v>
       </c>
     </row>
@@ -7552,16 +7624,16 @@
     </row>
     <row r="73" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A73" s="11"/>
-      <c r="B73" s="38"/>
-      <c r="C73" s="38">
+      <c r="B73" s="36"/>
+      <c r="C73" s="36">
         <v>-0.27600000000000002</v>
       </c>
-      <c r="D73" s="38"/>
-      <c r="E73" s="38">
+      <c r="D73" s="36"/>
+      <c r="E73" s="36">
         <v>-8.1539999999999999</v>
       </c>
-      <c r="F73" s="38"/>
-      <c r="G73" s="38">
+      <c r="F73" s="36"/>
+      <c r="G73" s="36">
         <v>-7.7560000000000002</v>
       </c>
     </row>
@@ -7584,16 +7656,16 @@
     </row>
     <row r="75" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A75" s="11"/>
-      <c r="B75" s="38"/>
-      <c r="C75" s="38">
+      <c r="B75" s="36"/>
+      <c r="C75" s="36">
         <v>-0.746</v>
       </c>
-      <c r="D75" s="38"/>
-      <c r="E75" s="38">
+      <c r="D75" s="36"/>
+      <c r="E75" s="36">
         <v>-18.603999999999999</v>
       </c>
-      <c r="F75" s="38"/>
-      <c r="G75" s="38">
+      <c r="F75" s="36"/>
+      <c r="G75" s="36">
         <v>-3.5760000000000001</v>
       </c>
     </row>
@@ -7616,29 +7688,29 @@
     </row>
     <row r="77" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A77" s="11"/>
-      <c r="B77" s="38"/>
-      <c r="C77" s="38">
+      <c r="B77" s="36"/>
+      <c r="C77" s="36">
         <v>-0.21299999999999999</v>
       </c>
-      <c r="D77" s="38"/>
-      <c r="E77" s="38">
+      <c r="D77" s="36"/>
+      <c r="E77" s="36">
         <v>-5.7709999999999999</v>
       </c>
-      <c r="F77" s="38"/>
-      <c r="G77" s="38">
+      <c r="F77" s="36"/>
+      <c r="G77" s="36">
         <v>-4.8490000000000002</v>
       </c>
     </row>
     <row r="78" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A78" s="11"/>
-      <c r="B78" s="31" t="s">
+      <c r="B78" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="31"/>
-      <c r="F78" s="31"/>
-      <c r="G78" s="31"/>
+      <c r="C78" s="40"/>
+      <c r="D78" s="40"/>
+      <c r="E78" s="40"/>
+      <c r="F78" s="40"/>
+      <c r="G78" s="40"/>
     </row>
     <row r="79" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1" thickBot="1">
       <c r="A79" s="11"/>
@@ -7648,16 +7720,16 @@
       <c r="C79" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D79" s="41" t="s">
+      <c r="D79" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E79" s="41" t="s">
+      <c r="E79" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F79" s="41" t="s">
+      <c r="F79" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="G79" s="41" t="s">
+      <c r="G79" s="39" t="s">
         <v>81</v>
       </c>
     </row>
@@ -7667,10 +7739,10 @@
       </c>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="37"/>
-      <c r="F80" s="37"/>
-      <c r="G80" s="37"/>
+      <c r="D80" s="35"/>
+      <c r="E80" s="35"/>
+      <c r="F80" s="35"/>
+      <c r="G80" s="35"/>
     </row>
     <row r="81" spans="1:7" ht="16" customHeight="1">
       <c r="A81" s="9" t="s">
@@ -7691,16 +7763,16 @@
     </row>
     <row r="82" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A82" s="11"/>
-      <c r="B82" s="38"/>
-      <c r="C82" s="38">
+      <c r="B82" s="36"/>
+      <c r="C82" s="36">
         <v>-0.14199999999999999</v>
       </c>
-      <c r="D82" s="38"/>
-      <c r="E82" s="38">
+      <c r="D82" s="36"/>
+      <c r="E82" s="36">
         <v>-3.5139999999999998</v>
       </c>
-      <c r="F82" s="38"/>
-      <c r="G82" s="38">
+      <c r="F82" s="36"/>
+      <c r="G82" s="36">
         <v>-2.6789999999999998</v>
       </c>
     </row>
@@ -7723,16 +7795,16 @@
     </row>
     <row r="84" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A84" s="11"/>
-      <c r="B84" s="38"/>
-      <c r="C84" s="38">
+      <c r="B84" s="36"/>
+      <c r="C84" s="36">
         <v>-7.8E-2</v>
       </c>
-      <c r="D84" s="38"/>
-      <c r="E84" s="38">
+      <c r="D84" s="36"/>
+      <c r="E84" s="36">
         <v>-2.0110000000000001</v>
       </c>
-      <c r="F84" s="38"/>
-      <c r="G84" s="38">
+      <c r="F84" s="36"/>
+      <c r="G84" s="36">
         <v>-1.5149999999999999</v>
       </c>
     </row>
@@ -7755,16 +7827,16 @@
     </row>
     <row r="86" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A86" s="11"/>
-      <c r="B86" s="38"/>
-      <c r="C86" s="38">
+      <c r="B86" s="36"/>
+      <c r="C86" s="36">
         <v>-0.16800000000000001</v>
       </c>
-      <c r="D86" s="38"/>
-      <c r="E86" s="38">
+      <c r="D86" s="36"/>
+      <c r="E86" s="36">
         <v>-3.7970000000000002</v>
       </c>
-      <c r="F86" s="38"/>
-      <c r="G86" s="38">
+      <c r="F86" s="36"/>
+      <c r="G86" s="36">
         <v>-2.7320000000000002</v>
       </c>
     </row>
@@ -7787,16 +7859,16 @@
     </row>
     <row r="88" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A88" s="11"/>
-      <c r="B88" s="38"/>
-      <c r="C88" s="38">
+      <c r="B88" s="36"/>
+      <c r="C88" s="36">
         <v>-8.6999999999999994E-2</v>
       </c>
-      <c r="D88" s="38"/>
-      <c r="E88" s="38">
+      <c r="D88" s="36"/>
+      <c r="E88" s="36">
         <v>-2.1840000000000002</v>
       </c>
-      <c r="F88" s="38"/>
-      <c r="G88" s="38">
+      <c r="F88" s="36"/>
+      <c r="G88" s="36">
         <v>-1.5049999999999999</v>
       </c>
     </row>
@@ -7819,16 +7891,16 @@
     </row>
     <row r="90" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A90" s="11"/>
-      <c r="B90" s="38"/>
-      <c r="C90" s="38">
+      <c r="B90" s="36"/>
+      <c r="C90" s="36">
         <v>-0.17899999999999999</v>
       </c>
-      <c r="D90" s="38"/>
-      <c r="E90" s="38">
+      <c r="D90" s="36"/>
+      <c r="E90" s="36">
         <v>-4.194</v>
       </c>
-      <c r="F90" s="38"/>
-      <c r="G90" s="38">
+      <c r="F90" s="36"/>
+      <c r="G90" s="36">
         <v>-3.004</v>
       </c>
     </row>
@@ -7851,16 +7923,16 @@
     </row>
     <row r="92" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A92" s="11"/>
-      <c r="B92" s="38"/>
-      <c r="C92" s="38">
+      <c r="B92" s="36"/>
+      <c r="C92" s="36">
         <v>-9.8000000000000004E-2</v>
       </c>
-      <c r="D92" s="38"/>
-      <c r="E92" s="38">
+      <c r="D92" s="36"/>
+      <c r="E92" s="36">
         <v>-2.641</v>
       </c>
-      <c r="F92" s="38"/>
-      <c r="G92" s="38">
+      <c r="F92" s="36"/>
+      <c r="G92" s="36">
         <v>-1.847</v>
       </c>
     </row>
@@ -7870,10 +7942,10 @@
       </c>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
-      <c r="D93" s="37"/>
-      <c r="E93" s="37"/>
-      <c r="F93" s="37"/>
-      <c r="G93" s="37"/>
+      <c r="D93" s="35"/>
+      <c r="E93" s="35"/>
+      <c r="F93" s="35"/>
+      <c r="G93" s="35"/>
     </row>
     <row r="94" spans="1:7" ht="16" customHeight="1">
       <c r="A94" s="9" t="s">
@@ -7894,16 +7966,16 @@
     </row>
     <row r="95" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A95" s="11"/>
-      <c r="B95" s="38"/>
-      <c r="C95" s="38">
+      <c r="B95" s="36"/>
+      <c r="C95" s="36">
         <v>-0.161</v>
       </c>
-      <c r="D95" s="38"/>
-      <c r="E95" s="38">
+      <c r="D95" s="36"/>
+      <c r="E95" s="36">
         <v>-4.1779999999999999</v>
       </c>
-      <c r="F95" s="38"/>
-      <c r="G95" s="38">
+      <c r="F95" s="36"/>
+      <c r="G95" s="36">
         <v>-3.4980000000000002</v>
       </c>
     </row>
@@ -7926,16 +7998,16 @@
     </row>
     <row r="97" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A97" s="11"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="38">
+      <c r="B97" s="36"/>
+      <c r="C97" s="36">
         <v>-0.09</v>
       </c>
-      <c r="D97" s="38"/>
-      <c r="E97" s="38">
+      <c r="D97" s="36"/>
+      <c r="E97" s="36">
         <v>-2.383</v>
       </c>
-      <c r="F97" s="38"/>
-      <c r="G97" s="38">
+      <c r="F97" s="36"/>
+      <c r="G97" s="36">
         <v>-1.994</v>
       </c>
     </row>
@@ -7958,16 +8030,16 @@
     </row>
     <row r="99" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A99" s="11"/>
-      <c r="B99" s="38"/>
-      <c r="C99" s="38">
+      <c r="B99" s="36"/>
+      <c r="C99" s="36">
         <v>-0.20499999999999999</v>
       </c>
-      <c r="D99" s="38"/>
-      <c r="E99" s="38">
+      <c r="D99" s="36"/>
+      <c r="E99" s="36">
         <v>-5.1050000000000004</v>
       </c>
-      <c r="F99" s="38"/>
-      <c r="G99" s="38">
+      <c r="F99" s="36"/>
+      <c r="G99" s="36">
         <v>-4.5039999999999996</v>
       </c>
     </row>
@@ -7990,16 +8062,16 @@
     </row>
     <row r="101" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A101" s="11"/>
-      <c r="B101" s="38"/>
-      <c r="C101" s="38">
+      <c r="B101" s="36"/>
+      <c r="C101" s="36">
         <v>-0.10299999999999999</v>
       </c>
-      <c r="D101" s="38"/>
-      <c r="E101" s="38">
+      <c r="D101" s="36"/>
+      <c r="E101" s="36">
         <v>-2.8439999999999999</v>
       </c>
-      <c r="F101" s="38"/>
-      <c r="G101" s="38">
+      <c r="F101" s="36"/>
+      <c r="G101" s="36">
         <v>-2.3119999999999998</v>
       </c>
     </row>
@@ -8022,16 +8094,16 @@
     </row>
     <row r="103" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A103" s="11"/>
-      <c r="B103" s="38"/>
-      <c r="C103" s="38">
+      <c r="B103" s="36"/>
+      <c r="C103" s="36">
         <v>-0.29299999999999998</v>
       </c>
-      <c r="D103" s="38"/>
-      <c r="E103" s="38">
+      <c r="D103" s="36"/>
+      <c r="E103" s="36">
         <v>-7.2389999999999999</v>
       </c>
-      <c r="F103" s="38"/>
-      <c r="G103" s="38">
+      <c r="F103" s="36"/>
+      <c r="G103" s="36">
         <v>-6.1580000000000004</v>
       </c>
     </row>
@@ -8054,16 +8126,16 @@
     </row>
     <row r="105" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A105" s="11"/>
-      <c r="B105" s="38"/>
-      <c r="C105" s="38">
+      <c r="B105" s="36"/>
+      <c r="C105" s="36">
         <v>-0.153</v>
       </c>
-      <c r="D105" s="38"/>
-      <c r="E105" s="38">
+      <c r="D105" s="36"/>
+      <c r="E105" s="36">
         <v>-4.1900000000000004</v>
       </c>
-      <c r="F105" s="38"/>
-      <c r="G105" s="38">
+      <c r="F105" s="36"/>
+      <c r="G105" s="36">
         <v>-3.8130000000000002</v>
       </c>
     </row>
@@ -8086,16 +8158,16 @@
     </row>
     <row r="107" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A107" s="11"/>
-      <c r="B107" s="38"/>
-      <c r="C107" s="38">
+      <c r="B107" s="36"/>
+      <c r="C107" s="36">
         <v>-0.255</v>
       </c>
-      <c r="D107" s="38"/>
-      <c r="E107" s="38">
+      <c r="D107" s="36"/>
+      <c r="E107" s="36">
         <v>-6.726</v>
       </c>
-      <c r="F107" s="38"/>
-      <c r="G107" s="38">
+      <c r="F107" s="36"/>
+      <c r="G107" s="36">
         <v>-5.149</v>
       </c>
     </row>
@@ -8118,16 +8190,16 @@
     </row>
     <row r="109" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A109" s="11"/>
-      <c r="B109" s="38"/>
-      <c r="C109" s="38">
+      <c r="B109" s="36"/>
+      <c r="C109" s="36">
         <v>-0.14699999999999999</v>
       </c>
-      <c r="D109" s="38"/>
-      <c r="E109" s="38">
+      <c r="D109" s="36"/>
+      <c r="E109" s="36">
         <v>-4.1120000000000001</v>
       </c>
-      <c r="F109" s="38"/>
-      <c r="G109" s="38">
+      <c r="F109" s="36"/>
+      <c r="G109" s="36">
         <v>-3.3490000000000002</v>
       </c>
     </row>
@@ -8150,16 +8222,16 @@
     </row>
     <row r="111" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A111" s="11"/>
-      <c r="B111" s="38"/>
-      <c r="C111" s="38">
+      <c r="B111" s="36"/>
+      <c r="C111" s="36">
         <v>-0.316</v>
       </c>
-      <c r="D111" s="38"/>
-      <c r="E111" s="38">
+      <c r="D111" s="36"/>
+      <c r="E111" s="36">
         <v>-8.0549999999999997</v>
       </c>
-      <c r="F111" s="38"/>
-      <c r="G111" s="38">
+      <c r="F111" s="36"/>
+      <c r="G111" s="36">
         <v>-6.6269999999999998</v>
       </c>
     </row>
@@ -8182,16 +8254,16 @@
     </row>
     <row r="113" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A113" s="11"/>
-      <c r="B113" s="38"/>
-      <c r="C113" s="38">
+      <c r="B113" s="36"/>
+      <c r="C113" s="36">
         <v>-0.183</v>
       </c>
-      <c r="D113" s="38"/>
-      <c r="E113" s="38">
+      <c r="D113" s="36"/>
+      <c r="E113" s="36">
         <v>-4.8179999999999996</v>
       </c>
-      <c r="F113" s="38"/>
-      <c r="G113" s="38">
+      <c r="F113" s="36"/>
+      <c r="G113" s="36">
         <v>-4.0279999999999996</v>
       </c>
     </row>
@@ -8214,16 +8286,16 @@
     </row>
     <row r="115" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A115" s="11"/>
-      <c r="B115" s="38"/>
-      <c r="C115" s="38">
+      <c r="B115" s="36"/>
+      <c r="C115" s="36">
         <v>-0.441</v>
       </c>
-      <c r="D115" s="38"/>
-      <c r="E115" s="38">
+      <c r="D115" s="36"/>
+      <c r="E115" s="36">
         <v>-10.944000000000001</v>
       </c>
-      <c r="F115" s="38"/>
-      <c r="G115" s="38">
+      <c r="F115" s="36"/>
+      <c r="G115" s="36">
         <v>-12.445</v>
       </c>
     </row>
@@ -8246,16 +8318,16 @@
     </row>
     <row r="117" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A117" s="11"/>
-      <c r="B117" s="38"/>
-      <c r="C117" s="38">
+      <c r="B117" s="36"/>
+      <c r="C117" s="36">
         <v>-0.23400000000000001</v>
       </c>
-      <c r="D117" s="38"/>
-      <c r="E117" s="38">
+      <c r="D117" s="36"/>
+      <c r="E117" s="36">
         <v>-8.1780000000000008</v>
       </c>
-      <c r="F117" s="38"/>
-      <c r="G117" s="38">
+      <c r="F117" s="36"/>
+      <c r="G117" s="36">
         <v>-6.9459999999999997</v>
       </c>
     </row>
@@ -8278,16 +8350,16 @@
     </row>
     <row r="119" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A119" s="11"/>
-      <c r="B119" s="38"/>
-      <c r="C119" s="38">
+      <c r="B119" s="36"/>
+      <c r="C119" s="36">
         <v>-0.36199999999999999</v>
       </c>
-      <c r="D119" s="38"/>
-      <c r="E119" s="38">
+      <c r="D119" s="36"/>
+      <c r="E119" s="36">
         <v>-12.53</v>
       </c>
-      <c r="F119" s="38"/>
-      <c r="G119" s="38">
+      <c r="F119" s="36"/>
+      <c r="G119" s="36">
         <v>-8.6859999999999999</v>
       </c>
     </row>
@@ -8310,16 +8382,16 @@
     </row>
     <row r="121" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A121" s="11"/>
-      <c r="B121" s="38"/>
-      <c r="C121" s="38">
+      <c r="B121" s="36"/>
+      <c r="C121" s="36">
         <v>-0.34200000000000003</v>
       </c>
-      <c r="D121" s="38"/>
-      <c r="E121" s="38">
+      <c r="D121" s="36"/>
+      <c r="E121" s="36">
         <v>-10.622</v>
       </c>
-      <c r="F121" s="38"/>
-      <c r="G121" s="38">
+      <c r="F121" s="36"/>
+      <c r="G121" s="36">
         <v>-7.835</v>
       </c>
     </row>
@@ -8342,16 +8414,16 @@
     </row>
     <row r="123" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A123" s="11"/>
-      <c r="B123" s="38"/>
-      <c r="C123" s="38">
+      <c r="B123" s="36"/>
+      <c r="C123" s="36">
         <v>-0.42199999999999999</v>
       </c>
-      <c r="D123" s="38"/>
-      <c r="E123" s="38">
+      <c r="D123" s="36"/>
+      <c r="E123" s="36">
         <v>-12.288</v>
       </c>
-      <c r="F123" s="38"/>
-      <c r="G123" s="38">
+      <c r="F123" s="36"/>
+      <c r="G123" s="36">
         <v>-8.1020000000000003</v>
       </c>
     </row>
@@ -8374,16 +8446,16 @@
     </row>
     <row r="125" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A125" s="11"/>
-      <c r="B125" s="38"/>
-      <c r="C125" s="38">
+      <c r="B125" s="36"/>
+      <c r="C125" s="36">
         <v>-0.35899999999999999</v>
       </c>
-      <c r="D125" s="38"/>
-      <c r="E125" s="38">
+      <c r="D125" s="36"/>
+      <c r="E125" s="36">
         <v>-12.654</v>
       </c>
-      <c r="F125" s="38"/>
-      <c r="G125" s="38">
+      <c r="F125" s="36"/>
+      <c r="G125" s="36">
         <v>-8.8119999999999994</v>
       </c>
     </row>
@@ -8406,16 +8478,16 @@
     </row>
     <row r="127" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A127" s="11"/>
-      <c r="B127" s="38"/>
-      <c r="C127" s="38">
+      <c r="B127" s="36"/>
+      <c r="C127" s="36">
         <v>-0.29899999999999999</v>
       </c>
-      <c r="D127" s="38"/>
-      <c r="E127" s="38">
+      <c r="D127" s="36"/>
+      <c r="E127" s="36">
         <v>-8.8949999999999996</v>
       </c>
-      <c r="F127" s="38"/>
-      <c r="G127" s="38">
+      <c r="F127" s="36"/>
+      <c r="G127" s="36">
         <v>-5.1680000000000001</v>
       </c>
     </row>
@@ -8424,22 +8496,22 @@
         <v>250</v>
       </c>
       <c r="B128" s="26"/>
-      <c r="C128" s="33" t="s">
+      <c r="C128" s="31" t="s">
         <v>251</v>
       </c>
       <c r="D128" s="18"/>
-      <c r="E128" s="33" t="s">
+      <c r="E128" s="31" t="s">
         <v>251</v>
       </c>
       <c r="F128" s="18"/>
-      <c r="G128" s="33" t="s">
+      <c r="G128" s="31" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="129" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A129" s="11"/>
-      <c r="B129" s="38"/>
-      <c r="C129" s="38"/>
+      <c r="B129" s="36"/>
+      <c r="C129" s="36"/>
       <c r="D129" s="18"/>
       <c r="E129" s="18"/>
       <c r="F129" s="18"/>
@@ -8464,16 +8536,16 @@
     </row>
     <row r="131" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A131" s="11"/>
-      <c r="B131" s="38"/>
-      <c r="C131" s="38">
+      <c r="B131" s="36"/>
+      <c r="C131" s="36">
         <v>-0.76300000000000001</v>
       </c>
-      <c r="D131" s="38"/>
-      <c r="E131" s="38">
+      <c r="D131" s="36"/>
+      <c r="E131" s="36">
         <v>-14.933999999999999</v>
       </c>
-      <c r="F131" s="38"/>
-      <c r="G131" s="38">
+      <c r="F131" s="36"/>
+      <c r="G131" s="36">
         <v>-11.750999999999999</v>
       </c>
     </row>
@@ -8496,16 +8568,16 @@
     </row>
     <row r="133" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A133" s="11"/>
-      <c r="B133" s="38"/>
-      <c r="C133" s="38">
+      <c r="B133" s="36"/>
+      <c r="C133" s="36">
         <v>-0.34100000000000003</v>
       </c>
-      <c r="D133" s="38"/>
-      <c r="E133" s="38">
+      <c r="D133" s="36"/>
+      <c r="E133" s="36">
         <v>-10.516</v>
       </c>
-      <c r="F133" s="38"/>
-      <c r="G133" s="38">
+      <c r="F133" s="36"/>
+      <c r="G133" s="36">
         <v>-7.6680000000000001</v>
       </c>
     </row>
@@ -8528,16 +8600,16 @@
     </row>
     <row r="135" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A135" s="11"/>
-      <c r="B135" s="38"/>
-      <c r="C135" s="38">
+      <c r="B135" s="36"/>
+      <c r="C135" s="36">
         <v>-0.58899999999999997</v>
       </c>
-      <c r="D135" s="38"/>
-      <c r="E135" s="38">
+      <c r="D135" s="36"/>
+      <c r="E135" s="36">
         <v>-17.306000000000001</v>
       </c>
-      <c r="F135" s="38"/>
-      <c r="G135" s="38">
+      <c r="F135" s="36"/>
+      <c r="G135" s="36">
         <v>-16.233000000000001</v>
       </c>
     </row>
@@ -8560,16 +8632,16 @@
     </row>
     <row r="137" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A137" s="11"/>
-      <c r="B137" s="38"/>
-      <c r="C137" s="38">
+      <c r="B137" s="36"/>
+      <c r="C137" s="36">
         <v>-0.34399999999999997</v>
       </c>
-      <c r="D137" s="38"/>
-      <c r="E137" s="38">
+      <c r="D137" s="36"/>
+      <c r="E137" s="36">
         <v>-12.74</v>
       </c>
-      <c r="F137" s="38"/>
-      <c r="G137" s="38">
+      <c r="F137" s="36"/>
+      <c r="G137" s="36">
         <v>-9.5030000000000001</v>
       </c>
     </row>
@@ -8592,16 +8664,16 @@
     </row>
     <row r="139" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A139" s="11"/>
-      <c r="B139" s="38"/>
-      <c r="C139" s="38">
+      <c r="B139" s="36"/>
+      <c r="C139" s="36">
         <v>-0.747</v>
       </c>
-      <c r="D139" s="38"/>
-      <c r="E139" s="38">
+      <c r="D139" s="36"/>
+      <c r="E139" s="36">
         <v>-12.534000000000001</v>
       </c>
-      <c r="F139" s="38"/>
-      <c r="G139" s="38">
+      <c r="F139" s="36"/>
+      <c r="G139" s="36">
         <v>-13.388999999999999</v>
       </c>
     </row>
@@ -8624,16 +8696,16 @@
     </row>
     <row r="141" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A141" s="11"/>
-      <c r="B141" s="38"/>
-      <c r="C141" s="38">
+      <c r="B141" s="36"/>
+      <c r="C141" s="36">
         <v>-0.313</v>
       </c>
-      <c r="D141" s="38"/>
-      <c r="E141" s="38">
+      <c r="D141" s="36"/>
+      <c r="E141" s="36">
         <v>-9.157</v>
       </c>
-      <c r="F141" s="38"/>
-      <c r="G141" s="38">
+      <c r="F141" s="36"/>
+      <c r="G141" s="36">
         <v>-6.2329999999999997</v>
       </c>
     </row>
@@ -8656,16 +8728,16 @@
     </row>
     <row r="143" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A143" s="11"/>
-      <c r="B143" s="38"/>
-      <c r="C143" s="38">
+      <c r="B143" s="36"/>
+      <c r="C143" s="36">
         <v>-0.35</v>
       </c>
-      <c r="D143" s="38"/>
-      <c r="E143" s="38">
+      <c r="D143" s="36"/>
+      <c r="E143" s="36">
         <v>-11.167</v>
       </c>
-      <c r="F143" s="38"/>
-      <c r="G143" s="38">
+      <c r="F143" s="36"/>
+      <c r="G143" s="36">
         <v>-21.074999999999999</v>
       </c>
     </row>
@@ -8688,16 +8760,16 @@
     </row>
     <row r="145" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A145" s="11"/>
-      <c r="B145" s="38"/>
-      <c r="C145" s="38">
+      <c r="B145" s="36"/>
+      <c r="C145" s="36">
         <v>-0.43099999999999999</v>
       </c>
-      <c r="D145" s="38"/>
-      <c r="E145" s="38">
+      <c r="D145" s="36"/>
+      <c r="E145" s="36">
         <v>-12.103999999999999</v>
       </c>
-      <c r="F145" s="38"/>
-      <c r="G145" s="38">
+      <c r="F145" s="36"/>
+      <c r="G145" s="36">
         <v>-8.94</v>
       </c>
     </row>
@@ -8706,22 +8778,22 @@
         <v>252</v>
       </c>
       <c r="B146" s="26"/>
-      <c r="C146" s="33" t="s">
+      <c r="C146" s="31" t="s">
         <v>251</v>
       </c>
       <c r="D146" s="18"/>
-      <c r="E146" s="33" t="s">
+      <c r="E146" s="31" t="s">
         <v>251</v>
       </c>
       <c r="F146" s="18"/>
-      <c r="G146" s="33" t="s">
+      <c r="G146" s="31" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="147" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A147" s="11"/>
-      <c r="B147" s="38"/>
-      <c r="C147" s="38"/>
+      <c r="B147" s="36"/>
+      <c r="C147" s="36"/>
       <c r="D147" s="18"/>
       <c r="E147" s="18"/>
       <c r="F147" s="18"/>
@@ -8746,16 +8818,16 @@
     </row>
     <row r="149" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A149" s="11"/>
-      <c r="B149" s="38"/>
-      <c r="C149" s="38">
+      <c r="B149" s="36"/>
+      <c r="C149" s="36">
         <v>-0.88</v>
       </c>
-      <c r="D149" s="38"/>
-      <c r="E149" s="38">
+      <c r="D149" s="36"/>
+      <c r="E149" s="36">
         <v>-22.152999999999999</v>
       </c>
-      <c r="F149" s="38"/>
-      <c r="G149" s="38">
+      <c r="F149" s="36"/>
+      <c r="G149" s="36">
         <v>-8.6349999999999998</v>
       </c>
     </row>
@@ -8764,22 +8836,22 @@
         <v>253</v>
       </c>
       <c r="B150" s="26"/>
-      <c r="C150" s="33" t="s">
+      <c r="C150" s="31" t="s">
         <v>251</v>
       </c>
       <c r="D150" s="18"/>
-      <c r="E150" s="33" t="s">
+      <c r="E150" s="31" t="s">
         <v>251</v>
       </c>
       <c r="F150" s="18"/>
-      <c r="G150" s="33" t="s">
+      <c r="G150" s="31" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="151" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A151" s="11"/>
-      <c r="B151" s="38"/>
-      <c r="C151" s="38"/>
+      <c r="B151" s="36"/>
+      <c r="C151" s="36"/>
       <c r="D151" s="18"/>
       <c r="E151" s="18"/>
       <c r="F151" s="18"/>
@@ -8804,29 +8876,29 @@
     </row>
     <row r="153" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A153" s="11"/>
-      <c r="B153" s="38"/>
-      <c r="C153" s="38">
+      <c r="B153" s="36"/>
+      <c r="C153" s="36">
         <v>-0.33700000000000002</v>
       </c>
-      <c r="D153" s="38"/>
-      <c r="E153" s="38">
+      <c r="D153" s="36"/>
+      <c r="E153" s="36">
         <v>-12.192</v>
       </c>
-      <c r="F153" s="38"/>
-      <c r="G153" s="38">
+      <c r="F153" s="36"/>
+      <c r="G153" s="36">
         <v>-7.782</v>
       </c>
     </row>
     <row r="154" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A154" s="11"/>
-      <c r="B154" s="31" t="s">
+      <c r="B154" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C154" s="31"/>
-      <c r="D154" s="31"/>
-      <c r="E154" s="31"/>
-      <c r="F154" s="31"/>
-      <c r="G154" s="31"/>
+      <c r="C154" s="40"/>
+      <c r="D154" s="40"/>
+      <c r="E154" s="40"/>
+      <c r="F154" s="40"/>
+      <c r="G154" s="40"/>
     </row>
     <row r="155" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1" thickBot="1">
       <c r="A155" s="11"/>
@@ -8836,16 +8908,16 @@
       <c r="C155" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D155" s="41" t="s">
+      <c r="D155" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E155" s="41" t="s">
+      <c r="E155" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F155" s="41" t="s">
+      <c r="F155" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="G155" s="41" t="s">
+      <c r="G155" s="39" t="s">
         <v>81</v>
       </c>
     </row>
@@ -8855,10 +8927,10 @@
       </c>
       <c r="B156" s="9"/>
       <c r="C156" s="9"/>
-      <c r="D156" s="37"/>
-      <c r="E156" s="37"/>
-      <c r="F156" s="37"/>
-      <c r="G156" s="37"/>
+      <c r="D156" s="35"/>
+      <c r="E156" s="35"/>
+      <c r="F156" s="35"/>
+      <c r="G156" s="35"/>
     </row>
     <row r="157" spans="1:7" ht="16" customHeight="1">
       <c r="A157" s="9" t="s">
@@ -8885,22 +8957,22 @@
     </row>
     <row r="158" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A158" s="11"/>
-      <c r="B158" s="38">
+      <c r="B158" s="36">
         <v>-1.6E-2</v>
       </c>
-      <c r="C158" s="38">
+      <c r="C158" s="36">
         <v>-1.6E-2</v>
       </c>
-      <c r="D158" s="38">
+      <c r="D158" s="36">
         <v>-0.375</v>
       </c>
-      <c r="E158" s="38">
+      <c r="E158" s="36">
         <v>-0.375</v>
       </c>
-      <c r="F158" s="38">
+      <c r="F158" s="36">
         <v>-0.32100000000000001</v>
       </c>
-      <c r="G158" s="38">
+      <c r="G158" s="36">
         <v>-0.32</v>
       </c>
     </row>
@@ -8910,10 +8982,10 @@
       </c>
       <c r="B159" s="9"/>
       <c r="C159" s="9"/>
-      <c r="D159" s="37"/>
-      <c r="E159" s="37"/>
-      <c r="F159" s="37"/>
-      <c r="G159" s="37"/>
+      <c r="D159" s="35"/>
+      <c r="E159" s="35"/>
+      <c r="F159" s="35"/>
+      <c r="G159" s="35"/>
     </row>
     <row r="160" spans="1:7" ht="16" customHeight="1">
       <c r="A160" s="10" t="s">
@@ -8940,22 +9012,22 @@
     </row>
     <row r="161" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A161" s="11"/>
-      <c r="B161" s="38">
+      <c r="B161" s="36">
         <v>-1.9E-2</v>
       </c>
-      <c r="C161" s="38">
+      <c r="C161" s="36">
         <v>-1.9E-2</v>
       </c>
-      <c r="D161" s="38">
+      <c r="D161" s="36">
         <v>-0.47799999999999998</v>
       </c>
-      <c r="E161" s="38">
+      <c r="E161" s="36">
         <v>-0.47899999999999998</v>
       </c>
-      <c r="F161" s="38">
+      <c r="F161" s="36">
         <v>-0.39400000000000002</v>
       </c>
-      <c r="G161" s="38">
+      <c r="G161" s="36">
         <v>-0.39500000000000002</v>
       </c>
     </row>
@@ -8984,22 +9056,22 @@
     </row>
     <row r="163" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A163" s="11"/>
-      <c r="B163" s="38">
+      <c r="B163" s="36">
         <v>-3.7999999999999999E-2</v>
       </c>
-      <c r="C163" s="38">
+      <c r="C163" s="36">
         <v>-3.7999999999999999E-2</v>
       </c>
-      <c r="D163" s="38">
+      <c r="D163" s="36">
         <v>-0.93100000000000005</v>
       </c>
-      <c r="E163" s="38">
+      <c r="E163" s="36">
         <v>-0.93300000000000005</v>
       </c>
-      <c r="F163" s="38">
+      <c r="F163" s="36">
         <v>-0.81200000000000006</v>
       </c>
-      <c r="G163" s="38">
+      <c r="G163" s="36">
         <v>-0.80700000000000005</v>
       </c>
     </row>
@@ -9009,10 +9081,10 @@
       </c>
       <c r="B164" s="9"/>
       <c r="C164" s="9"/>
-      <c r="D164" s="37"/>
-      <c r="E164" s="37"/>
-      <c r="F164" s="37"/>
-      <c r="G164" s="37"/>
+      <c r="D164" s="35"/>
+      <c r="E164" s="35"/>
+      <c r="F164" s="35"/>
+      <c r="G164" s="35"/>
     </row>
     <row r="165" spans="1:7" ht="16" customHeight="1">
       <c r="A165" s="9" t="s">
@@ -9039,22 +9111,22 @@
     </row>
     <row r="166" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A166" s="11"/>
-      <c r="B166" s="38">
+      <c r="B166" s="36">
         <v>-1.9E-2</v>
       </c>
-      <c r="C166" s="38">
+      <c r="C166" s="36">
         <v>-1.9E-2</v>
       </c>
-      <c r="D166" s="38">
+      <c r="D166" s="36">
         <v>-0.46700000000000003</v>
       </c>
-      <c r="E166" s="38">
+      <c r="E166" s="36">
         <v>-0.46800000000000003</v>
       </c>
-      <c r="F166" s="38">
+      <c r="F166" s="36">
         <v>-0.38100000000000001</v>
       </c>
-      <c r="G166" s="38">
+      <c r="G166" s="36">
         <v>-0.38100000000000001</v>
       </c>
     </row>
@@ -9083,22 +9155,22 @@
     </row>
     <row r="168" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A168" s="11"/>
-      <c r="B168" s="38">
+      <c r="B168" s="36">
         <v>-2.9000000000000001E-2</v>
       </c>
-      <c r="C168" s="38">
+      <c r="C168" s="36">
         <v>-2.9000000000000001E-2</v>
       </c>
-      <c r="D168" s="38">
+      <c r="D168" s="36">
         <v>-0.753</v>
       </c>
-      <c r="E168" s="38">
+      <c r="E168" s="36">
         <v>-0.754</v>
       </c>
-      <c r="F168" s="38">
+      <c r="F168" s="36">
         <v>-0.625</v>
       </c>
-      <c r="G168" s="38">
+      <c r="G168" s="36">
         <v>-0.625</v>
       </c>
     </row>
@@ -9127,22 +9199,22 @@
     </row>
     <row r="170" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A170" s="11"/>
-      <c r="B170" s="38">
+      <c r="B170" s="36">
         <v>-5.2999999999999999E-2</v>
       </c>
-      <c r="C170" s="38">
+      <c r="C170" s="36">
         <v>-7.1999999999999995E-2</v>
       </c>
-      <c r="D170" s="38">
+      <c r="D170" s="36">
         <v>-1.365</v>
       </c>
-      <c r="E170" s="38">
+      <c r="E170" s="36">
         <v>-1.929</v>
       </c>
-      <c r="F170" s="38">
+      <c r="F170" s="36">
         <v>-1.147</v>
       </c>
-      <c r="G170" s="38">
+      <c r="G170" s="36">
         <v>-1.603</v>
       </c>
     </row>
@@ -9152,10 +9224,10 @@
       </c>
       <c r="B171" s="9"/>
       <c r="C171" s="9"/>
-      <c r="D171" s="37"/>
-      <c r="E171" s="37"/>
-      <c r="F171" s="37"/>
-      <c r="G171" s="37"/>
+      <c r="D171" s="35"/>
+      <c r="E171" s="35"/>
+      <c r="F171" s="35"/>
+      <c r="G171" s="35"/>
     </row>
     <row r="172" spans="1:7" ht="16" customHeight="1">
       <c r="A172" s="9" t="s">
@@ -9182,22 +9254,22 @@
     </row>
     <row r="173" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A173" s="11"/>
-      <c r="B173" s="38">
+      <c r="B173" s="36">
         <v>-1.7999999999999999E-2</v>
       </c>
-      <c r="C173" s="38">
+      <c r="C173" s="36">
         <v>-1.7999999999999999E-2</v>
       </c>
-      <c r="D173" s="38">
+      <c r="D173" s="36">
         <v>-0.45100000000000001</v>
       </c>
-      <c r="E173" s="38">
+      <c r="E173" s="36">
         <v>-0.45</v>
       </c>
-      <c r="F173" s="38">
+      <c r="F173" s="36">
         <v>-0.377</v>
       </c>
-      <c r="G173" s="38">
+      <c r="G173" s="36">
         <v>-0.378</v>
       </c>
     </row>
@@ -9207,10 +9279,10 @@
       </c>
       <c r="B174" s="9"/>
       <c r="C174" s="9"/>
-      <c r="D174" s="37"/>
-      <c r="E174" s="37"/>
-      <c r="F174" s="37"/>
-      <c r="G174" s="37"/>
+      <c r="D174" s="35"/>
+      <c r="E174" s="35"/>
+      <c r="F174" s="35"/>
+      <c r="G174" s="35"/>
     </row>
     <row r="175" spans="1:7" ht="16" customHeight="1">
       <c r="A175" s="9" t="s">
@@ -9237,22 +9309,22 @@
     </row>
     <row r="176" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A176" s="11"/>
-      <c r="B176" s="38">
+      <c r="B176" s="36">
         <v>-1.4999999999999999E-2</v>
       </c>
-      <c r="C176" s="38">
+      <c r="C176" s="36">
         <v>-1.6E-2</v>
       </c>
-      <c r="D176" s="38">
+      <c r="D176" s="36">
         <v>-0.38800000000000001</v>
       </c>
-      <c r="E176" s="38">
+      <c r="E176" s="36">
         <v>-0.38800000000000001</v>
       </c>
-      <c r="F176" s="38">
+      <c r="F176" s="36">
         <v>-0.32500000000000001</v>
       </c>
-      <c r="G176" s="38">
+      <c r="G176" s="36">
         <v>-0.32600000000000001</v>
       </c>
     </row>
@@ -9262,10 +9334,10 @@
       </c>
       <c r="B177" s="9"/>
       <c r="C177" s="9"/>
-      <c r="D177" s="37"/>
-      <c r="E177" s="37"/>
-      <c r="F177" s="37"/>
-      <c r="G177" s="37"/>
+      <c r="D177" s="35"/>
+      <c r="E177" s="35"/>
+      <c r="F177" s="35"/>
+      <c r="G177" s="35"/>
     </row>
     <row r="178" spans="1:7" ht="16" customHeight="1">
       <c r="A178" s="9" t="s">
@@ -9292,22 +9364,22 @@
     </row>
     <row r="179" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A179" s="13"/>
-      <c r="B179" s="38">
+      <c r="B179" s="36">
         <v>-0.253</v>
       </c>
-      <c r="C179" s="38">
+      <c r="C179" s="36">
         <v>-0.255</v>
       </c>
-      <c r="D179" s="38">
+      <c r="D179" s="36">
         <v>-6.2069999999999999</v>
       </c>
-      <c r="E179" s="38">
+      <c r="E179" s="36">
         <v>-6.17</v>
       </c>
-      <c r="F179" s="38">
+      <c r="F179" s="36">
         <v>-4.8970000000000002</v>
       </c>
-      <c r="G179" s="38">
+      <c r="G179" s="36">
         <v>-5.0110000000000001</v>
       </c>
     </row>
@@ -9336,22 +9408,22 @@
     </row>
     <row r="181" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A181" s="13"/>
-      <c r="B181" s="38">
+      <c r="B181" s="36">
         <v>-2.1000000000000001E-2</v>
       </c>
-      <c r="C181" s="38">
+      <c r="C181" s="36">
         <v>-2.1000000000000001E-2</v>
       </c>
-      <c r="D181" s="38">
+      <c r="D181" s="36">
         <v>-0.502</v>
       </c>
-      <c r="E181" s="38">
+      <c r="E181" s="36">
         <v>-0.503</v>
       </c>
-      <c r="F181" s="38">
+      <c r="F181" s="36">
         <v>-0.42299999999999999</v>
       </c>
-      <c r="G181" s="38">
+      <c r="G181" s="36">
         <v>-0.42299999999999999</v>
       </c>
     </row>
@@ -9380,22 +9452,22 @@
     </row>
     <row r="183" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A183" s="13"/>
-      <c r="B183" s="38">
+      <c r="B183" s="36">
         <v>-2.5000000000000001E-2</v>
       </c>
-      <c r="C183" s="38">
+      <c r="C183" s="36">
         <v>-2.5000000000000001E-2</v>
       </c>
-      <c r="D183" s="38">
+      <c r="D183" s="36">
         <v>-0.58199999999999996</v>
       </c>
-      <c r="E183" s="38">
+      <c r="E183" s="36">
         <v>-0.58199999999999996</v>
       </c>
-      <c r="F183" s="38">
+      <c r="F183" s="36">
         <v>-0.498</v>
       </c>
-      <c r="G183" s="38">
+      <c r="G183" s="36">
         <v>-0.497</v>
       </c>
     </row>
@@ -9424,22 +9496,22 @@
     </row>
     <row r="185" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A185" s="13"/>
-      <c r="B185" s="38">
+      <c r="B185" s="36">
         <v>-2.7E-2</v>
       </c>
-      <c r="C185" s="38">
+      <c r="C185" s="36">
         <v>-2.7E-2</v>
       </c>
-      <c r="D185" s="38">
+      <c r="D185" s="36">
         <v>-0.63200000000000001</v>
       </c>
-      <c r="E185" s="38">
+      <c r="E185" s="36">
         <v>-0.63300000000000001</v>
       </c>
-      <c r="F185" s="38">
+      <c r="F185" s="36">
         <v>-0.53800000000000003</v>
       </c>
-      <c r="G185" s="38">
+      <c r="G185" s="36">
         <v>-0.53800000000000003</v>
       </c>
     </row>
@@ -9468,22 +9540,22 @@
     </row>
     <row r="187" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A187" s="13"/>
-      <c r="B187" s="38">
+      <c r="B187" s="36">
         <v>-3.4000000000000002E-2</v>
       </c>
-      <c r="C187" s="38">
+      <c r="C187" s="36">
         <v>-3.4000000000000002E-2</v>
       </c>
-      <c r="D187" s="38">
+      <c r="D187" s="36">
         <v>-0.81399999999999995</v>
       </c>
-      <c r="E187" s="38">
+      <c r="E187" s="36">
         <v>-0.81499999999999995</v>
       </c>
-      <c r="F187" s="38">
+      <c r="F187" s="36">
         <v>-0.68100000000000005</v>
       </c>
-      <c r="G187" s="38">
+      <c r="G187" s="36">
         <v>-0.68</v>
       </c>
     </row>
@@ -9512,22 +9584,22 @@
     </row>
     <row r="189" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A189" s="13"/>
-      <c r="B189" s="38">
+      <c r="B189" s="36">
         <v>-3.9E-2</v>
       </c>
-      <c r="C189" s="38">
+      <c r="C189" s="36">
         <v>-3.9E-2</v>
       </c>
-      <c r="D189" s="38">
+      <c r="D189" s="36">
         <v>-0.93500000000000005</v>
       </c>
-      <c r="E189" s="38">
+      <c r="E189" s="36">
         <v>-0.93300000000000005</v>
       </c>
-      <c r="F189" s="38">
+      <c r="F189" s="36">
         <v>-0.745</v>
       </c>
-      <c r="G189" s="38">
+      <c r="G189" s="36">
         <v>-0.748</v>
       </c>
     </row>
@@ -9556,22 +9628,22 @@
     </row>
     <row r="191" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A191" s="11"/>
-      <c r="B191" s="38">
+      <c r="B191" s="36">
         <v>-0.19600000000000001</v>
       </c>
-      <c r="C191" s="38">
+      <c r="C191" s="36">
         <v>-0.20200000000000001</v>
       </c>
-      <c r="D191" s="38">
+      <c r="D191" s="36">
         <v>-1.587</v>
       </c>
-      <c r="E191" s="38">
+      <c r="E191" s="36">
         <v>-1.5669999999999999</v>
       </c>
-      <c r="F191" s="38">
+      <c r="F191" s="36">
         <v>-6.2290000000000001</v>
       </c>
-      <c r="G191" s="38">
+      <c r="G191" s="36">
         <v>-6.3280000000000003</v>
       </c>
     </row>
@@ -9581,10 +9653,10 @@
       </c>
       <c r="B192" s="9"/>
       <c r="C192" s="9"/>
-      <c r="D192" s="37"/>
-      <c r="E192" s="37"/>
-      <c r="F192" s="37"/>
-      <c r="G192" s="37"/>
+      <c r="D192" s="35"/>
+      <c r="E192" s="35"/>
+      <c r="F192" s="35"/>
+      <c r="G192" s="35"/>
     </row>
     <row r="193" spans="1:7" ht="16" customHeight="1">
       <c r="A193" s="9" t="s">
@@ -9611,22 +9683,22 @@
     </row>
     <row r="194" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A194" s="11"/>
-      <c r="B194" s="38">
+      <c r="B194" s="36">
         <v>-1.9E-2</v>
       </c>
-      <c r="C194" s="38">
+      <c r="C194" s="36">
         <v>-1.9E-2</v>
       </c>
-      <c r="D194" s="38">
+      <c r="D194" s="36">
         <v>-0.42099999999999999</v>
       </c>
-      <c r="E194" s="38">
+      <c r="E194" s="36">
         <v>-0.42299999999999999</v>
       </c>
-      <c r="F194" s="38">
+      <c r="F194" s="36">
         <v>-0.33800000000000002</v>
       </c>
-      <c r="G194" s="38">
+      <c r="G194" s="36">
         <v>-0.33800000000000002</v>
       </c>
     </row>
@@ -9654,22 +9726,22 @@
       </c>
     </row>
     <row r="196" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
-      <c r="B196" s="38">
+      <c r="B196" s="36">
         <v>-0.14199999999999999</v>
       </c>
-      <c r="C196" s="38">
+      <c r="C196" s="36">
         <v>-0.14199999999999999</v>
       </c>
-      <c r="D196" s="38">
+      <c r="D196" s="36">
         <v>-3.5</v>
       </c>
-      <c r="E196" s="38">
+      <c r="E196" s="36">
         <v>-3.43</v>
       </c>
-      <c r="F196" s="38">
+      <c r="F196" s="36">
         <v>-2.6579999999999999</v>
       </c>
-      <c r="G196" s="38">
+      <c r="G196" s="36">
         <v>-2.6749999999999998</v>
       </c>
     </row>
@@ -9679,10 +9751,10 @@
       </c>
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
-      <c r="D197" s="37"/>
-      <c r="E197" s="37"/>
-      <c r="F197" s="37"/>
-      <c r="G197" s="37"/>
+      <c r="D197" s="35"/>
+      <c r="E197" s="35"/>
+      <c r="F197" s="35"/>
+      <c r="G197" s="35"/>
     </row>
     <row r="198" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A198" s="9" t="s">
@@ -9708,22 +9780,22 @@
       </c>
     </row>
     <row r="199" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
-      <c r="B199" s="38">
+      <c r="B199" s="36">
         <v>-1.6E-2</v>
       </c>
-      <c r="C199" s="38">
+      <c r="C199" s="36">
         <v>-1.6E-2</v>
       </c>
-      <c r="D199" s="38">
+      <c r="D199" s="36">
         <v>-0.40100000000000002</v>
       </c>
-      <c r="E199" s="38">
+      <c r="E199" s="36">
         <v>-0.40200000000000002</v>
       </c>
-      <c r="F199" s="38">
+      <c r="F199" s="36">
         <v>-0.33400000000000002</v>
       </c>
-      <c r="G199" s="38">
+      <c r="G199" s="36">
         <v>-0.33400000000000002</v>
       </c>
     </row>
@@ -9752,22 +9824,22 @@
     </row>
     <row r="201" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A201" s="11"/>
-      <c r="B201" s="38">
+      <c r="B201" s="36">
         <v>-2E-3</v>
       </c>
-      <c r="C201" s="38">
+      <c r="C201" s="36">
         <v>-2E-3</v>
       </c>
-      <c r="D201" s="38">
+      <c r="D201" s="36">
         <v>-5.1999999999999998E-2</v>
       </c>
-      <c r="E201" s="38">
+      <c r="E201" s="36">
         <v>-5.1999999999999998E-2</v>
       </c>
-      <c r="F201" s="38">
+      <c r="F201" s="36">
         <v>-0.04</v>
       </c>
-      <c r="G201" s="38">
+      <c r="G201" s="36">
         <v>-0.04</v>
       </c>
     </row>
@@ -9775,10 +9847,10 @@
       <c r="A202" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="B202" s="33" t="s">
+      <c r="B202" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="C202" s="33" t="s">
+      <c r="C202" s="31" t="s">
         <v>251</v>
       </c>
       <c r="D202" s="26" t="s">
@@ -9796,18 +9868,18 @@
     </row>
     <row r="203" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A203" s="11"/>
-      <c r="B203" s="39"/>
-      <c r="C203" s="39"/>
-      <c r="D203" s="38">
+      <c r="B203" s="37"/>
+      <c r="C203" s="37"/>
+      <c r="D203" s="36">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="E203" s="38">
+      <c r="E203" s="36">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="F203" s="38">
+      <c r="F203" s="36">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="G203" s="38">
+      <c r="G203" s="36">
         <v>-8.9999999999999993E-3</v>
       </c>
     </row>
@@ -9882,22 +9954,22 @@
     </row>
     <row r="207" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1" thickBot="1">
       <c r="A207" s="15"/>
-      <c r="B207" s="40">
+      <c r="B207" s="38">
         <v>-5.5E-2</v>
       </c>
-      <c r="C207" s="40">
+      <c r="C207" s="38">
         <v>-7.0999999999999994E-2</v>
       </c>
-      <c r="D207" s="40">
+      <c r="D207" s="38">
         <v>-1.3520000000000001</v>
       </c>
-      <c r="E207" s="40">
+      <c r="E207" s="38">
         <v>-1.7669999999999999</v>
       </c>
-      <c r="F207" s="40">
+      <c r="F207" s="38">
         <v>-1.111</v>
       </c>
-      <c r="G207" s="40">
+      <c r="G207" s="38">
         <v>-1.4</v>
       </c>
     </row>
@@ -9928,48 +10000,48 @@
       <c r="A209" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B209" s="35">
+      <c r="B209" s="33">
         <v>0.80056817016348902</v>
       </c>
-      <c r="C209" s="35">
+      <c r="C209" s="33">
         <v>0.80063857056295595</v>
       </c>
-      <c r="D209" s="35">
+      <c r="D209" s="33">
         <v>0.43521467448187601</v>
       </c>
-      <c r="E209" s="35">
+      <c r="E209" s="33">
         <v>0.43620907991729202</v>
       </c>
-      <c r="F209" s="35">
+      <c r="F209" s="33">
         <v>0.63838361026145096</v>
       </c>
-      <c r="G209" s="35">
+      <c r="G209" s="33">
         <v>0.639240259848604</v>
       </c>
     </row>
     <row r="210" spans="1:18" ht="16" customHeight="1">
       <c r="A210" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B210" s="34"/>
-      <c r="C210" s="34"/>
-    </row>
-    <row r="212" spans="1:18" ht="16" customHeight="1">
-      <c r="A212" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B210" s="32"/>
+      <c r="C210" s="32"/>
+    </row>
+    <row r="211" spans="1:18" ht="16" customHeight="1">
+      <c r="A211" s="6" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="217" spans="1:18" ht="16" customHeight="1">
-      <c r="L217" s="4"/>
-      <c r="M217" s="14"/>
-      <c r="N217" s="14"/>
-      <c r="O217" s="14"/>
-      <c r="P217" s="14"/>
-      <c r="Q217" s="14"/>
-      <c r="R217" s="14"/>
-    </row>
-    <row r="218" spans="1:18" ht="16" customHeight="1">
-      <c r="L218" s="36"/>
+    <row r="215" spans="1:18" ht="16" customHeight="1">
+      <c r="L215" s="4"/>
+      <c r="M215" s="14"/>
+      <c r="N215" s="14"/>
+      <c r="O215" s="14"/>
+      <c r="P215" s="14"/>
+      <c r="Q215" s="14"/>
+      <c r="R215" s="14"/>
+    </row>
+    <row r="216" spans="1:18" ht="16" customHeight="1">
+      <c r="L216" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9984,10 +10056,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA9308D-7049-0444-A25D-BC13BCC9D9DA}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="G66" sqref="A1:G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" customHeight="1"/>
@@ -9999,14 +10071,14 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" customHeight="1">
       <c r="A1" s="3"/>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1" thickBot="1">
       <c r="A2" s="19"/>
@@ -10016,16 +10088,16 @@
       <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="39" t="s">
         <v>81</v>
       </c>
     </row>
@@ -10061,22 +10133,22 @@
     </row>
     <row r="5" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A5" s="13"/>
-      <c r="B5" s="38">
+      <c r="B5" s="36">
         <v>-0.02</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="36">
         <v>-5.3999999999999999E-2</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="36">
         <v>-0.499</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="36">
         <v>-1.4690000000000001</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="36">
         <v>-0.52400000000000002</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="36">
         <v>-1.1919999999999999</v>
       </c>
     </row>
@@ -10086,10 +10158,10 @@
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
     </row>
     <row r="7" spans="1:7" ht="16" customHeight="1">
       <c r="A7" s="9" t="s">
@@ -10116,22 +10188,22 @@
     </row>
     <row r="8" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A8" s="11"/>
-      <c r="B8" s="38">
+      <c r="B8" s="36">
         <v>-2.9000000000000001E-2</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="36">
         <v>-0.105</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="36">
         <v>-0.77500000000000002</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="36">
         <v>-2.4300000000000002</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="36">
         <v>-0.68400000000000005</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G8" s="36">
         <v>-1.8779999999999999</v>
       </c>
     </row>
@@ -10160,22 +10232,22 @@
     </row>
     <row r="10" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A10" s="11"/>
-      <c r="B10" s="38">
+      <c r="B10" s="36">
         <v>-1.6E-2</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="36">
         <v>-5.5E-2</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="36">
         <v>-0.49</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="36">
         <v>-1.4279999999999999</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="36">
         <v>-0.42199999999999999</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="36">
         <v>-1.0309999999999999</v>
       </c>
     </row>
@@ -10185,8 +10257,8 @@
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
     </row>
@@ -10215,22 +10287,22 @@
     </row>
     <row r="13" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A13" s="11"/>
-      <c r="B13" s="38">
+      <c r="B13" s="36">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="36">
         <v>-7.1999999999999995E-2</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="36">
         <v>-0.441</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="36">
         <v>-1.859</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="36">
         <v>-0.38100000000000001</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G13" s="36">
         <v>-1.4119999999999999</v>
       </c>
     </row>
@@ -10259,22 +10331,22 @@
     </row>
     <row r="15" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="38">
+      <c r="B15" s="36">
         <v>-2.1000000000000001E-2</v>
       </c>
-      <c r="C15" s="38">
+      <c r="C15" s="36">
         <v>-8.1000000000000003E-2</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="36">
         <v>-0.53900000000000003</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="36">
         <v>-2.0379999999999998</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="36">
         <v>-0.45500000000000002</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G15" s="36">
         <v>-1.4239999999999999</v>
       </c>
     </row>
@@ -10303,22 +10375,22 @@
     </row>
     <row r="17" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A17" s="11"/>
-      <c r="B17" s="38">
+      <c r="B17" s="36">
         <v>-2.7E-2</v>
       </c>
-      <c r="C17" s="38">
+      <c r="C17" s="36">
         <v>-9.5000000000000001E-2</v>
       </c>
-      <c r="D17" s="38">
+      <c r="D17" s="36">
         <v>-0.63400000000000001</v>
       </c>
-      <c r="E17" s="38">
+      <c r="E17" s="36">
         <v>-2.5310000000000001</v>
       </c>
-      <c r="F17" s="38">
+      <c r="F17" s="36">
         <v>-0.51100000000000001</v>
       </c>
-      <c r="G17" s="38">
+      <c r="G17" s="36">
         <v>-1.7729999999999999</v>
       </c>
     </row>
@@ -10328,10 +10400,10 @@
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
     </row>
     <row r="19" spans="1:7" ht="16" customHeight="1">
       <c r="A19" s="9" t="s">
@@ -10352,16 +10424,16 @@
     </row>
     <row r="20" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A20" s="11"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38">
+      <c r="B20" s="36"/>
+      <c r="C20" s="36">
         <v>-0.114</v>
       </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38">
+      <c r="D20" s="36"/>
+      <c r="E20" s="36">
         <v>-2.762</v>
       </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38">
+      <c r="F20" s="36"/>
+      <c r="G20" s="36">
         <v>-2.3119999999999998</v>
       </c>
     </row>
@@ -10384,16 +10456,16 @@
     </row>
     <row r="22" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A22" s="11"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38">
+      <c r="B22" s="36"/>
+      <c r="C22" s="36">
         <v>-6.0999999999999999E-2</v>
       </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38">
+      <c r="D22" s="36"/>
+      <c r="E22" s="36">
         <v>-1.6339999999999999</v>
       </c>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38">
+      <c r="F22" s="36"/>
+      <c r="G22" s="36">
         <v>-1.296</v>
       </c>
     </row>
@@ -10403,10 +10475,10 @@
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
     </row>
     <row r="24" spans="1:7" ht="16" customHeight="1">
       <c r="A24" s="9" t="s">
@@ -10427,16 +10499,16 @@
     </row>
     <row r="25" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A25" s="11"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38">
+      <c r="B25" s="36"/>
+      <c r="C25" s="36">
         <v>-7.9000000000000001E-2</v>
       </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38">
+      <c r="D25" s="36"/>
+      <c r="E25" s="36">
         <v>-2.0960000000000001</v>
       </c>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38">
+      <c r="F25" s="36"/>
+      <c r="G25" s="36">
         <v>-1.7290000000000001</v>
       </c>
     </row>
@@ -10459,16 +10531,16 @@
     </row>
     <row r="27" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A27" s="11"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38">
+      <c r="B27" s="36"/>
+      <c r="C27" s="36">
         <v>-9.0999999999999998E-2</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38">
+      <c r="D27" s="36"/>
+      <c r="E27" s="36">
         <v>-2.5459999999999998</v>
       </c>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38">
+      <c r="F27" s="36"/>
+      <c r="G27" s="36">
         <v>-2.0350000000000001</v>
       </c>
     </row>
@@ -10491,16 +10563,16 @@
     </row>
     <row r="29" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A29" s="11"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38">
+      <c r="B29" s="36"/>
+      <c r="C29" s="36">
         <v>-0.14099999999999999</v>
       </c>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38">
+      <c r="D29" s="36"/>
+      <c r="E29" s="36">
         <v>-3.8460000000000001</v>
       </c>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38">
+      <c r="F29" s="36"/>
+      <c r="G29" s="36">
         <v>-3.5190000000000001</v>
       </c>
     </row>
@@ -10510,10 +10582,10 @@
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
     </row>
     <row r="31" spans="1:7" ht="16" customHeight="1">
       <c r="A31" s="9" t="s">
@@ -10534,16 +10606,16 @@
     </row>
     <row r="32" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A32" s="11"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38">
+      <c r="B32" s="36"/>
+      <c r="C32" s="36">
         <v>-0.14199999999999999</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38">
+      <c r="D32" s="36"/>
+      <c r="E32" s="36">
         <v>-3.5139999999999998</v>
       </c>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38">
+      <c r="F32" s="36"/>
+      <c r="G32" s="36">
         <v>-2.6789999999999998</v>
       </c>
     </row>
@@ -10566,16 +10638,16 @@
     </row>
     <row r="34" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A34" s="11"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38">
+      <c r="B34" s="36"/>
+      <c r="C34" s="36">
         <v>-7.8E-2</v>
       </c>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38">
+      <c r="D34" s="36"/>
+      <c r="E34" s="36">
         <v>-2.0110000000000001</v>
       </c>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38">
+      <c r="F34" s="36"/>
+      <c r="G34" s="36">
         <v>-1.5149999999999999</v>
       </c>
     </row>
@@ -10598,16 +10670,16 @@
     </row>
     <row r="36" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A36" s="11"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38">
+      <c r="B36" s="36"/>
+      <c r="C36" s="36">
         <v>-0.16800000000000001</v>
       </c>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38">
+      <c r="D36" s="36"/>
+      <c r="E36" s="36">
         <v>-3.7970000000000002</v>
       </c>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38">
+      <c r="F36" s="36"/>
+      <c r="G36" s="36">
         <v>-2.7320000000000002</v>
       </c>
     </row>
@@ -10630,16 +10702,16 @@
     </row>
     <row r="38" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A38" s="11"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38">
+      <c r="B38" s="36"/>
+      <c r="C38" s="36">
         <v>-8.6999999999999994E-2</v>
       </c>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38">
+      <c r="D38" s="36"/>
+      <c r="E38" s="36">
         <v>-2.1840000000000002</v>
       </c>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38">
+      <c r="F38" s="36"/>
+      <c r="G38" s="36">
         <v>-1.5049999999999999</v>
       </c>
     </row>
@@ -10662,16 +10734,16 @@
     </row>
     <row r="40" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A40" s="11"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38">
+      <c r="B40" s="36"/>
+      <c r="C40" s="36">
         <v>-0.17899999999999999</v>
       </c>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38">
+      <c r="D40" s="36"/>
+      <c r="E40" s="36">
         <v>-4.194</v>
       </c>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38">
+      <c r="F40" s="36"/>
+      <c r="G40" s="36">
         <v>-3.004</v>
       </c>
     </row>
@@ -10694,16 +10766,16 @@
     </row>
     <row r="42" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A42" s="11"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38">
+      <c r="B42" s="36"/>
+      <c r="C42" s="36">
         <v>-9.8000000000000004E-2</v>
       </c>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38">
+      <c r="D42" s="36"/>
+      <c r="E42" s="36">
         <v>-2.641</v>
       </c>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38">
+      <c r="F42" s="36"/>
+      <c r="G42" s="36">
         <v>-1.847</v>
       </c>
     </row>
@@ -10713,10 +10785,10 @@
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
     </row>
     <row r="44" spans="1:7" ht="16" customHeight="1">
       <c r="A44" s="9" t="s">
@@ -10737,16 +10809,16 @@
     </row>
     <row r="45" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A45" s="11"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38">
+      <c r="B45" s="36"/>
+      <c r="C45" s="36">
         <v>-0.161</v>
       </c>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38">
+      <c r="D45" s="36"/>
+      <c r="E45" s="36">
         <v>-4.1779999999999999</v>
       </c>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38">
+      <c r="F45" s="36"/>
+      <c r="G45" s="36">
         <v>-3.4980000000000002</v>
       </c>
     </row>
@@ -10769,16 +10841,16 @@
     </row>
     <row r="47" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A47" s="11"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38">
+      <c r="B47" s="36"/>
+      <c r="C47" s="36">
         <v>-0.09</v>
       </c>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38">
+      <c r="D47" s="36"/>
+      <c r="E47" s="36">
         <v>-2.383</v>
       </c>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38">
+      <c r="F47" s="36"/>
+      <c r="G47" s="36">
         <v>-1.994</v>
       </c>
     </row>
@@ -10801,16 +10873,16 @@
     </row>
     <row r="49" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A49" s="11"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38">
+      <c r="B49" s="36"/>
+      <c r="C49" s="36">
         <v>-0.20499999999999999</v>
       </c>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38">
+      <c r="D49" s="36"/>
+      <c r="E49" s="36">
         <v>-5.1050000000000004</v>
       </c>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38">
+      <c r="F49" s="36"/>
+      <c r="G49" s="36">
         <v>-4.5039999999999996</v>
       </c>
     </row>
@@ -10833,16 +10905,16 @@
     </row>
     <row r="51" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A51" s="11"/>
-      <c r="B51" s="38"/>
-      <c r="C51" s="38">
+      <c r="B51" s="36"/>
+      <c r="C51" s="36">
         <v>-0.10299999999999999</v>
       </c>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38">
+      <c r="D51" s="36"/>
+      <c r="E51" s="36">
         <v>-2.8439999999999999</v>
       </c>
-      <c r="F51" s="38"/>
-      <c r="G51" s="38">
+      <c r="F51" s="36"/>
+      <c r="G51" s="36">
         <v>-2.3119999999999998</v>
       </c>
     </row>
@@ -10865,16 +10937,16 @@
     </row>
     <row r="53" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A53" s="11"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38">
+      <c r="B53" s="36"/>
+      <c r="C53" s="36">
         <v>-0.29299999999999998</v>
       </c>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38">
+      <c r="D53" s="36"/>
+      <c r="E53" s="36">
         <v>-7.2389999999999999</v>
       </c>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38">
+      <c r="F53" s="36"/>
+      <c r="G53" s="36">
         <v>-6.1580000000000004</v>
       </c>
     </row>
@@ -10897,16 +10969,16 @@
     </row>
     <row r="55" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A55" s="11"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="38">
+      <c r="B55" s="36"/>
+      <c r="C55" s="36">
         <v>-0.153</v>
       </c>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38">
+      <c r="D55" s="36"/>
+      <c r="E55" s="36">
         <v>-4.1900000000000004</v>
       </c>
-      <c r="F55" s="38"/>
-      <c r="G55" s="38">
+      <c r="F55" s="36"/>
+      <c r="G55" s="36">
         <v>-3.8130000000000002</v>
       </c>
     </row>
@@ -10937,10 +11009,10 @@
       <c r="A57" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="B57" s="33" t="s">
+      <c r="B57" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="C57" s="33" t="s">
+      <c r="C57" s="31" t="s">
         <v>251</v>
       </c>
       <c r="D57" s="26" t="s">
@@ -10958,18 +11030,18 @@
     </row>
     <row r="58" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1">
       <c r="A58" s="11"/>
-      <c r="B58" s="39"/>
-      <c r="C58" s="39"/>
-      <c r="D58" s="38">
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="36">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="E58" s="38">
+      <c r="E58" s="36">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="F58" s="38">
+      <c r="F58" s="36">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="G58" s="38">
+      <c r="G58" s="36">
         <v>-8.9999999999999993E-3</v>
       </c>
     </row>
@@ -11044,22 +11116,22 @@
     </row>
     <row r="62" spans="1:7" s="12" customFormat="1" ht="16" customHeight="1" thickBot="1">
       <c r="A62" s="15"/>
-      <c r="B62" s="40">
+      <c r="B62" s="38">
         <v>-5.5E-2</v>
       </c>
-      <c r="C62" s="40">
+      <c r="C62" s="38">
         <v>-7.0999999999999994E-2</v>
       </c>
-      <c r="D62" s="40">
+      <c r="D62" s="38">
         <v>-1.3520000000000001</v>
       </c>
-      <c r="E62" s="40">
+      <c r="E62" s="38">
         <v>-1.7669999999999999</v>
       </c>
-      <c r="F62" s="40">
+      <c r="F62" s="38">
         <v>-1.111</v>
       </c>
-      <c r="G62" s="40">
+      <c r="G62" s="38">
         <v>-1.4</v>
       </c>
     </row>
@@ -11090,31 +11162,36 @@
       <c r="A64" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="35">
+      <c r="B64" s="33">
         <v>0.80056817016348902</v>
       </c>
-      <c r="C64" s="35">
+      <c r="C64" s="33">
         <v>0.80063857056295595</v>
       </c>
-      <c r="D64" s="35">
+      <c r="D64" s="33">
         <v>0.43521467448187601</v>
       </c>
-      <c r="E64" s="35">
+      <c r="E64" s="33">
         <v>0.43620907991729202</v>
       </c>
-      <c r="F64" s="35">
+      <c r="F64" s="33">
         <v>0.63838361026145096</v>
       </c>
-      <c r="G64" s="35">
+      <c r="G64" s="33">
         <v>0.639240259848604</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="16" customHeight="1">
-      <c r="A65" s="36" t="s">
-        <v>311</v>
-      </c>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
+      <c r="A65" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="B65" s="32"/>
+      <c r="C65" s="32"/>
+    </row>
+    <row r="66" spans="1:3" ht="16" customHeight="1">
+      <c r="A66" s="6" t="s">
+        <v>313</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>